<commit_message>
excel data source files udpates
</commit_message>
<xml_diff>
--- a/data2019/abudhabi2019.xlsx
+++ b/data2019/abudhabi2019.xlsx
@@ -1,25 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Year 5\COMP 4801 FYP\codes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Year 5\COMP 4801 FYP\codes\data2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D4F86F-AC70-455E-8B79-8599C64D47F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ED81C3-C83D-4979-8185-92EACC05E347}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{25909279-3FED-49C2-85F2-F1BD41911B2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="8" xr2:uid="{25909279-3FED-49C2-85F2-F1BD41911B2F}"/>
   </bookViews>
   <sheets>
     <sheet name="fastestlap" sheetId="3" r:id="rId1"/>
     <sheet name="lapchart" sheetId="1" r:id="rId2"/>
     <sheet name="laptimes" sheetId="8" r:id="rId3"/>
-    <sheet name="pitstop" sheetId="2" r:id="rId4"/>
-    <sheet name="totallaptimes" sheetId="9" r:id="rId5"/>
+    <sheet name="totallaptimes" sheetId="9" r:id="rId4"/>
+    <sheet name="pitstop" sheetId="2" r:id="rId5"/>
     <sheet name="lapdelta" sheetId="10" r:id="rId6"/>
     <sheet name="lapsundercut" sheetId="11" r:id="rId7"/>
+    <sheet name="weather" sheetId="14" r:id="rId8"/>
+    <sheet name="altitude" sheetId="15" r:id="rId9"/>
+    <sheet name="finalstanding" sheetId="13" r:id="rId10"/>
+    <sheet name="integrated" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="132">
   <si>
     <t>Pos.</t>
   </si>
@@ -378,16 +382,98 @@
   <si>
     <t>delta_position</t>
   </si>
+  <si>
+    <t>tyre_before</t>
+  </si>
+  <si>
+    <t>tyre_after</t>
+  </si>
+  <si>
+    <t>final_pos</t>
+  </si>
+  <si>
+    <t>Pos</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>DNF</t>
+  </si>
+  <si>
+    <t>final_pos_gained</t>
+  </si>
+  <si>
+    <t>final_points</t>
+  </si>
+  <si>
+    <t>initial_pos</t>
+  </si>
+  <si>
+    <t>no_of_pits</t>
+  </si>
+  <si>
+    <t>laps_travelled</t>
+  </si>
+  <si>
+    <t>tyre_grid</t>
+  </si>
+  <si>
+    <t>tyre_1</t>
+  </si>
+  <si>
+    <t>tyre_2</t>
+  </si>
+  <si>
+    <t>tyre_grid_distance</t>
+  </si>
+  <si>
+    <t>tyre_1_distance</t>
+  </si>
+  <si>
+    <t>tyre_2_distance</t>
+  </si>
+  <si>
+    <t>Skycondition</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>79.77°F</t>
+  </si>
+  <si>
+    <t>Humidity</t>
+  </si>
+  <si>
+    <t>Wind speed</t>
+  </si>
+  <si>
+    <t>9.07 mph</t>
+  </si>
+  <si>
+    <t>Wind bearing</t>
+  </si>
+  <si>
+    <t>330°</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="mm:ss.000"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss.000"/>
+    <numFmt numFmtId="166" formatCode="h:mm:ss.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,16 +481,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -412,17 +522,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -738,7 +872,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G21"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,11 +1372,1023 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26D98304-78C6-4441-B29A-934F8866B9A0}">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>44</v>
+      </c>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>77</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>23</v>
+      </c>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>26</v>
+      </c>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>55</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>27</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>99</v>
+      </c>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>63</v>
+      </c>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>88</v>
+      </c>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="K21" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9768B7BF-17E8-4A06-86B3-7F23C0B7186B}">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <f>MATCH(A2,lapchart!B2:U2,0)</f>
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A2,finalstanding!B:B,0))</f>
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <f>IFERROR(C2-B2,"DNF")</f>
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <f>IF(C2=1,25,IF(C2=2,18,IF(C2=3,15,IF(C2=4,12,IF(C2=5,10,IF(C2=6,8,IF(C2=7,6,IF(C2=8,4,IF(C2=9,2,IF(C2=10,1,0))))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIF(pitstop!A:A, A2)</f>
+        <v>2</v>
+      </c>
+      <c r="J2" cm="1">
+        <f t="array" ref="J2">IF(F2&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A2=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>11</v>
+      </c>
+      <c r="K2" cm="1">
+        <f t="array" ref="K2">IF(F2&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J2,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A2=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>31</v>
+      </c>
+      <c r="L2" cm="1">
+        <f t="array" ref="L2">IF(F2&lt;3,IF(F2=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K2),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A2=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <f>MATCH(A3,lapchart!B3:U3,0)</f>
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A3,finalstanding!B:B,0))</f>
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D21" si="0">IFERROR(C3-B3,"DNF")</f>
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E21" si="1">IF(C3=1,25,IF(C3=2,18,IF(C3=3,15,IF(C3=4,12,IF(C3=5,10,IF(C3=6,8,IF(C3=7,6,IF(C3=8,4,IF(C3=9,2,IF(C3=10,1,0))))))))))</f>
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <f>COUNTIF(pitstop!A:A, A3)</f>
+        <v>1</v>
+      </c>
+      <c r="J3" cm="1">
+        <f t="array" ref="J3">IF(F3&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A3=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>8</v>
+      </c>
+      <c r="K3" cm="1">
+        <f t="array" ref="K3">IF(F3&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J3,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A3=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>47</v>
+      </c>
+      <c r="L3" t="str" cm="1">
+        <f t="array" ref="L3">IF(F3&lt;3,IF(F3=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K3),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A3=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <f>MATCH(A4,lapchart!B4:U4,0)</f>
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A4,finalstanding!B:B,0))</f>
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <f>COUNTIF(pitstop!A:A, A4)</f>
+        <v>2</v>
+      </c>
+      <c r="J4" cm="1">
+        <f t="array" ref="J4">IF(F4&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A4=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>12</v>
+      </c>
+      <c r="K4" cm="1">
+        <f t="array" ref="K4">IF(F4&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J4,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A4=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>26</v>
+      </c>
+      <c r="L4" cm="1">
+        <f t="array" ref="L4">IF(F4&lt;3,IF(F4=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K4),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A4=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>MATCH(A5,lapchart!B5:U5,0)</f>
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A5,finalstanding!B:B,0))</f>
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f>COUNTIF(pitstop!A:A, A5)</f>
+        <v>1</v>
+      </c>
+      <c r="J5" cm="1">
+        <f t="array" ref="J5">IF(F5&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A5=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>22</v>
+      </c>
+      <c r="K5" cm="1">
+        <f t="array" ref="K5">IF(F5&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J5,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A5=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>33</v>
+      </c>
+      <c r="L5" t="str" cm="1">
+        <f t="array" ref="L5">IF(F5&lt;3,IF(F5=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K5),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A5=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>MATCH(A6,lapchart!B6:U6,0)</f>
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A6,finalstanding!B:B,0))</f>
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f>COUNTIF(pitstop!A:A, A6)</f>
+        <v>1</v>
+      </c>
+      <c r="J6" cm="1">
+        <f t="array" ref="J6">IF(F6&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A6=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>18</v>
+      </c>
+      <c r="K6" cm="1">
+        <f t="array" ref="K6">IF(F6&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J6,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A6=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>37</v>
+      </c>
+      <c r="L6" t="str" cm="1">
+        <f t="array" ref="L6">IF(F6&lt;3,IF(F6=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K6),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A6=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <f>MATCH(A7,lapchart!B7:U7,0)</f>
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A7,finalstanding!B:B,0))</f>
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f>COUNTIF(pitstop!A:A, A7)</f>
+        <v>1</v>
+      </c>
+      <c r="J7" cm="1">
+        <f t="array" ref="J7">IF(F7&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A7=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>1</v>
+      </c>
+      <c r="K7" cm="1">
+        <f t="array" ref="K7">IF(F7&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J7,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A7=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>54</v>
+      </c>
+      <c r="L7" t="str" cm="1">
+        <f t="array" ref="L7">IF(F7&lt;3,IF(F7=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K7),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A7=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <f>MATCH(A8,lapchart!B8:U8,0)</f>
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A8,finalstanding!B:B,0))</f>
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <f>COUNTIF(pitstop!A:A, A8)</f>
+        <v>1</v>
+      </c>
+      <c r="J8" cm="1">
+        <f t="array" ref="J8">IF(F8&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A8=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>37</v>
+      </c>
+      <c r="K8" cm="1">
+        <f t="array" ref="K8">IF(F8&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J8,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A8=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>18</v>
+      </c>
+      <c r="L8" t="str" cm="1">
+        <f t="array" ref="L8">IF(F8&lt;3,IF(F8=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K8),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A8=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <f>MATCH(A9,lapchart!B9:U9,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A9,finalstanding!B:B,0))</f>
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <f>COUNTIF(pitstop!A:A, A9)</f>
+        <v>2</v>
+      </c>
+      <c r="J9" cm="1">
+        <f t="array" ref="J9">IF(F9&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A9=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>12</v>
+      </c>
+      <c r="K9" cm="1">
+        <f t="array" ref="K9">IF(F9&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J9,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A9=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>26</v>
+      </c>
+      <c r="L9" cm="1">
+        <f t="array" ref="L9">IF(F9&lt;3,IF(F9=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K9),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A9=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <f>MATCH(A10,lapchart!B10:U10,0)</f>
+        <v>19</v>
+      </c>
+      <c r="C10" t="str">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A10,finalstanding!B:B,0))</f>
+        <v>DNF</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>DNF</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f>COUNTIF(pitstop!A:A, A10)</f>
+        <v>2</v>
+      </c>
+      <c r="J10" cm="1">
+        <f t="array" ref="J10">IF(F10&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A10=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>5</v>
+      </c>
+      <c r="K10" cm="1">
+        <f t="array" ref="K10">IF(F10&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J10,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A10=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>18</v>
+      </c>
+      <c r="L10" cm="1">
+        <f t="array" ref="L10">IF(F10&lt;3,IF(F10=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K10),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A10=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <f>MATCH(A11,lapchart!B11:U11,0)</f>
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A11,finalstanding!B:B,0))</f>
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f>COUNTIF(pitstop!A:A, A11)</f>
+        <v>1</v>
+      </c>
+      <c r="J11" cm="1">
+        <f t="array" ref="J11">IF(F11&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A11=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>20</v>
+      </c>
+      <c r="K11" cm="1">
+        <f t="array" ref="K11">IF(F11&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J11,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A11=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>35</v>
+      </c>
+      <c r="L11" t="str" cm="1">
+        <f t="array" ref="L11">IF(F11&lt;3,IF(F11=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K11),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A11=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <f>MATCH(A12,lapchart!B12:U12,0)</f>
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A12,finalstanding!B:B,0))</f>
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <f>COUNTIF(pitstop!A:A, A12)</f>
+        <v>1</v>
+      </c>
+      <c r="J12" cm="1">
+        <f t="array" ref="J12">IF(F12&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A12=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>13</v>
+      </c>
+      <c r="K12" cm="1">
+        <f t="array" ref="K12">IF(F12&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J12,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A12=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>42</v>
+      </c>
+      <c r="L12" t="str" cm="1">
+        <f t="array" ref="L12">IF(F12&lt;3,IF(F12=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K12),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A12=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <f>MATCH(A13,lapchart!B13:U13,0)</f>
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A13,finalstanding!B:B,0))</f>
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <f>COUNTIF(pitstop!A:A, A13)</f>
+        <v>1</v>
+      </c>
+      <c r="J13" cm="1">
+        <f t="array" ref="J13">IF(F13&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A13=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>40</v>
+      </c>
+      <c r="K13" cm="1">
+        <f t="array" ref="K13">IF(F13&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J13,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A13=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>15</v>
+      </c>
+      <c r="L13" t="str" cm="1">
+        <f t="array" ref="L13">IF(F13&lt;3,IF(F13=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K13),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A13=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <f>MATCH(A14,lapchart!B14:U14,0)</f>
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A14,finalstanding!B:B,0))</f>
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f>COUNTIF(pitstop!A:A, A14)</f>
+        <v>1</v>
+      </c>
+      <c r="J14" cm="1">
+        <f t="array" ref="J14">IF(F14&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A14=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>18</v>
+      </c>
+      <c r="K14" cm="1">
+        <f t="array" ref="K14">IF(F14&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J14,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A14=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>37</v>
+      </c>
+      <c r="L14" t="str" cm="1">
+        <f t="array" ref="L14">IF(F14&lt;3,IF(F14=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K14),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A14=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>33</v>
+      </c>
+      <c r="B15">
+        <f>MATCH(A15,lapchart!B15:U15,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A15,finalstanding!B:B,0))</f>
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="F15">
+        <f>COUNTIF(pitstop!A:A, A15)</f>
+        <v>1</v>
+      </c>
+      <c r="J15" cm="1">
+        <f t="array" ref="J15">IF(F15&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A15=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>25</v>
+      </c>
+      <c r="K15" cm="1">
+        <f t="array" ref="K15">IF(F15&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J15,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A15=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>30</v>
+      </c>
+      <c r="L15" t="str" cm="1">
+        <f t="array" ref="L15">IF(F15&lt;3,IF(F15=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K15),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A15=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>44</v>
+      </c>
+      <c r="B16">
+        <f>MATCH(A16,lapchart!B16:U16,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A16,finalstanding!B:B,0))</f>
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="F16">
+        <f>COUNTIF(pitstop!A:A, A16)</f>
+        <v>1</v>
+      </c>
+      <c r="J16" cm="1">
+        <f t="array" ref="J16">IF(F16&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A16=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>26</v>
+      </c>
+      <c r="K16" cm="1">
+        <f t="array" ref="K16">IF(F16&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J16,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A16=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>29</v>
+      </c>
+      <c r="L16" t="str" cm="1">
+        <f t="array" ref="L16">IF(F16&lt;3,IF(F16=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K16),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A16=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>55</v>
+      </c>
+      <c r="B17">
+        <f>MATCH(A17,lapchart!B17:U17,0)</f>
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A17,finalstanding!B:B,0))</f>
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f>COUNTIF(pitstop!A:A, A17)</f>
+        <v>2</v>
+      </c>
+      <c r="J17" cm="1">
+        <f t="array" ref="J17">IF(F17&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A17=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>12</v>
+      </c>
+      <c r="K17" cm="1">
+        <f t="array" ref="K17">IF(F17&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J17,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A17=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>29</v>
+      </c>
+      <c r="L17" cm="1">
+        <f t="array" ref="L17">IF(F17&lt;3,IF(F17=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K17),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A17=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>63</v>
+      </c>
+      <c r="B18">
+        <f>MATCH(A18,lapchart!B18:U18,0)</f>
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A18,finalstanding!B:B,0))</f>
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f>COUNTIF(pitstop!A:A, A18)</f>
+        <v>1</v>
+      </c>
+      <c r="J18" cm="1">
+        <f t="array" ref="J18">IF(F18&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A18=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>32</v>
+      </c>
+      <c r="K18" cm="1">
+        <f t="array" ref="K18">IF(F18&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J18,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A18=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>23</v>
+      </c>
+      <c r="L18" t="str" cm="1">
+        <f t="array" ref="L18">IF(F18&lt;3,IF(F18=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K18),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A18=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>77</v>
+      </c>
+      <c r="B19">
+        <f>MATCH(A19,lapchart!B19:U19,0)</f>
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A19,finalstanding!B:B,0))</f>
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <f>COUNTIF(pitstop!A:A, A19)</f>
+        <v>1</v>
+      </c>
+      <c r="J19" cm="1">
+        <f t="array" ref="J19">IF(F19&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A19=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>29</v>
+      </c>
+      <c r="K19" cm="1">
+        <f t="array" ref="K19">IF(F19&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J19,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A19=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>26</v>
+      </c>
+      <c r="L19" t="str" cm="1">
+        <f t="array" ref="L19">IF(F19&lt;3,IF(F19=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K19),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A19=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>88</v>
+      </c>
+      <c r="B20">
+        <f>MATCH(A20,lapchart!B20:U20,0)</f>
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A20,finalstanding!B:B,0))</f>
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f>COUNTIF(pitstop!A:A, A20)</f>
+        <v>1</v>
+      </c>
+      <c r="J20" cm="1">
+        <f t="array" ref="J20">IF(F20&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A20=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>24</v>
+      </c>
+      <c r="K20" cm="1">
+        <f t="array" ref="K20">IF(F20&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J20,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A20=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>31</v>
+      </c>
+      <c r="L20" t="str" cm="1">
+        <f t="array" ref="L20">IF(F20&lt;3,IF(F20=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K20),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A20=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>99</v>
+      </c>
+      <c r="B21">
+        <f>MATCH(A21,lapchart!B21:U21,0)</f>
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <f>INDEX(finalstanding!A:A,MATCH(integrated!A21,finalstanding!B:B,0))</f>
+        <v>16</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f>COUNTIF(pitstop!A:A, A21)</f>
+        <v>2</v>
+      </c>
+      <c r="J21" cm="1">
+        <f t="array" ref="J21">IF(F21&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A21=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
+        <v>8</v>
+      </c>
+      <c r="K21" cm="1">
+        <f t="array" ref="K21">IF(F21&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J21,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A21=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
+        <v>18</v>
+      </c>
+      <c r="L21" cm="1">
+        <f t="array" ref="L21">IF(F21&lt;3,IF(F21=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K21),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A21=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F0C22B-C035-46D0-BF18-D4B9460A3AFE}">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4889,8 +6035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C50D7A4-D497-4764-8623-DC89CAFAC117}">
   <dimension ref="A1:V79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8907,652 +10053,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18896F0-13FF-4F21-9D1E-CDC6EE342C8B}">
-  <dimension ref="A1:G27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2">
-        <v>11</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>21.904</v>
-      </c>
-      <c r="G2">
-        <v>21.904</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3">
-        <v>42</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>21.623999999999999</v>
-      </c>
-      <c r="G3">
-        <v>21.623999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>22.974</v>
-      </c>
-      <c r="G4">
-        <v>22.974</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>25.771000000000001</v>
-      </c>
-      <c r="G5">
-        <v>25.771000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6">
-        <v>38</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>21.858000000000001</v>
-      </c>
-      <c r="G6">
-        <v>21.858000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7">
-        <v>22</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>22.41</v>
-      </c>
-      <c r="G7">
-        <v>22.41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8">
-        <v>18</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>21.968</v>
-      </c>
-      <c r="G8">
-        <v>21.968</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>8.9660879629629628E-4</v>
-      </c>
-      <c r="G9" s="1">
-        <v>8.9660879629629628E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10">
-        <v>37</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>22.23</v>
-      </c>
-      <c r="G10">
-        <v>22.23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11">
-        <v>12</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>21.696999999999999</v>
-      </c>
-      <c r="G11">
-        <v>21.696999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12">
-        <v>38</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12">
-        <v>21.274000000000001</v>
-      </c>
-      <c r="G12">
-        <v>21.274000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>28.841999999999999</v>
-      </c>
-      <c r="G13">
-        <v>28.841999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14">
-        <v>23</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-      <c r="F14">
-        <v>21.777999999999999</v>
-      </c>
-      <c r="G14">
-        <v>21.777999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15">
-        <v>20</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>21.530999999999999</v>
-      </c>
-      <c r="G15">
-        <v>21.530999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16">
-        <v>13</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>22.027999999999999</v>
-      </c>
-      <c r="G16">
-        <v>22.027999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17">
-        <v>40</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>21.495999999999999</v>
-      </c>
-      <c r="G17">
-        <v>21.495999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>27</v>
-      </c>
-      <c r="B18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18">
-        <v>18</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>21.577999999999999</v>
-      </c>
-      <c r="G18">
-        <v>21.577999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19">
-        <v>25</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>21.023</v>
-      </c>
-      <c r="G19">
-        <v>21.023</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>44</v>
-      </c>
-      <c r="B20" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20">
-        <v>26</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>22.178000000000001</v>
-      </c>
-      <c r="G20">
-        <v>22.178000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>55</v>
-      </c>
-      <c r="B21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21">
-        <v>12</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>21.928000000000001</v>
-      </c>
-      <c r="G21">
-        <v>21.928000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>55</v>
-      </c>
-      <c r="B22" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22">
-        <v>41</v>
-      </c>
-      <c r="E22">
-        <v>2</v>
-      </c>
-      <c r="F22">
-        <v>21.466000000000001</v>
-      </c>
-      <c r="G22">
-        <v>21.466000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>63</v>
-      </c>
-      <c r="B23" t="s">
-        <v>85</v>
-      </c>
-      <c r="C23" t="s">
-        <v>86</v>
-      </c>
-      <c r="D23">
-        <v>32</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>22.271999999999998</v>
-      </c>
-      <c r="G23">
-        <v>22.271999999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>77</v>
-      </c>
-      <c r="B24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24">
-        <v>29</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>21.145</v>
-      </c>
-      <c r="G24">
-        <v>21.145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>88</v>
-      </c>
-      <c r="B25" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25">
-        <v>24</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>21.687999999999999</v>
-      </c>
-      <c r="G25">
-        <v>21.687999999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>99</v>
-      </c>
-      <c r="B26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26">
-        <v>8</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>21.977</v>
-      </c>
-      <c r="G26">
-        <v>21.977</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>99</v>
-      </c>
-      <c r="B27" t="s">
-        <v>89</v>
-      </c>
-      <c r="C27" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27">
-        <v>26</v>
-      </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-      <c r="F27">
-        <v>22.187999999999999</v>
-      </c>
-      <c r="G27">
-        <v>22.187999999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A798E155-A830-4855-9A5E-DE730D057525}">
   <dimension ref="A1:U59"/>
   <sheetViews>
@@ -14378,18 +14878,938 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18896F0-13FF-4F21-9D1E-CDC6EE342C8B}">
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>21.904</v>
+      </c>
+      <c r="G2">
+        <v>21.904</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <f>IF(E2&gt;1,D2-D1,D2)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3">
+        <v>42</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>21.623999999999999</v>
+      </c>
+      <c r="G3">
+        <v>21.623999999999999</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J27" si="0">IF(E3&gt;1,D3-D2,D3)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>22.974</v>
+      </c>
+      <c r="G4">
+        <v>22.974</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>25.771000000000001</v>
+      </c>
+      <c r="G5">
+        <v>25.771000000000001</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6">
+        <v>38</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>21.858000000000001</v>
+      </c>
+      <c r="G6">
+        <v>21.858000000000001</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>22.41</v>
+      </c>
+      <c r="G7">
+        <v>22.41</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>21.968</v>
+      </c>
+      <c r="G8">
+        <v>21.968</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>8.9660879629629628E-4</v>
+      </c>
+      <c r="G9" s="1">
+        <v>8.9660879629629628E-4</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10">
+        <v>37</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>22.23</v>
+      </c>
+      <c r="G10">
+        <v>22.23</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>21.696999999999999</v>
+      </c>
+      <c r="G11">
+        <v>21.696999999999999</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12">
+        <v>38</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>21.274000000000001</v>
+      </c>
+      <c r="G12">
+        <v>21.274000000000001</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>28.841999999999999</v>
+      </c>
+      <c r="G13">
+        <v>28.841999999999999</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14">
+        <v>23</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>21.777999999999999</v>
+      </c>
+      <c r="G14">
+        <v>21.777999999999999</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>21.530999999999999</v>
+      </c>
+      <c r="G15">
+        <v>21.530999999999999</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16">
+        <v>13</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>22.027999999999999</v>
+      </c>
+      <c r="G16">
+        <v>22.027999999999999</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17">
+        <v>40</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>21.495999999999999</v>
+      </c>
+      <c r="G17">
+        <v>21.495999999999999</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18">
+        <v>18</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>21.577999999999999</v>
+      </c>
+      <c r="G18">
+        <v>21.577999999999999</v>
+      </c>
+      <c r="H18">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19">
+        <v>25</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>21.023</v>
+      </c>
+      <c r="G19">
+        <v>21.023</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20">
+        <v>26</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>22.178000000000001</v>
+      </c>
+      <c r="G20">
+        <v>22.178000000000001</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21">
+        <v>12</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>21.928000000000001</v>
+      </c>
+      <c r="G21">
+        <v>21.928000000000001</v>
+      </c>
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22">
+        <v>41</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>21.466000000000001</v>
+      </c>
+      <c r="G22">
+        <v>21.466000000000001</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23">
+        <v>32</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>22.271999999999998</v>
+      </c>
+      <c r="G23">
+        <v>22.271999999999998</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+      <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>77</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>21.145</v>
+      </c>
+      <c r="G24">
+        <v>21.145</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>88</v>
+      </c>
+      <c r="B25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25">
+        <v>24</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>21.687999999999999</v>
+      </c>
+      <c r="G25">
+        <v>21.687999999999999</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+      <c r="I25">
+        <v>4</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>99</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>21.977</v>
+      </c>
+      <c r="G26">
+        <v>21.977</v>
+      </c>
+      <c r="H26">
+        <v>5</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>99</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27">
+        <v>26</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>22.187999999999999</v>
+      </c>
+      <c r="G27">
+        <v>22.187999999999999</v>
+      </c>
+      <c r="H27">
+        <v>3</v>
+      </c>
+      <c r="I27">
+        <v>4</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD3ECFB-7C72-4F47-BC3F-BEDAF7778EC2}">
   <dimension ref="A1:U60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="21" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="13" max="21" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -19364,8 +20784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A8BBA3-10D4-484D-8976-742AE906AB2F}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20067,4 +21487,87 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF1F72E-23CB-4059-9281-935AB9D8E0EA}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462B709E-4F89-4A2D-8419-CE543F9C2CEC}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1">
+        <v>10.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Post final presentation update
</commit_message>
<xml_diff>
--- a/data2019/abudhabi2019.xlsx
+++ b/data2019/abudhabi2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Year 5\COMP 4801 FYP\codes\data2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ED81C3-C83D-4979-8185-92EACC05E347}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565B65F2-5404-4FE9-A5FA-CF1DF921E3C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="8" xr2:uid="{25909279-3FED-49C2-85F2-F1BD41911B2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="11" xr2:uid="{25909279-3FED-49C2-85F2-F1BD41911B2F}"/>
   </bookViews>
   <sheets>
     <sheet name="fastestlap" sheetId="3" r:id="rId1"/>
@@ -19,11 +19,13 @@
     <sheet name="totallaptimes" sheetId="9" r:id="rId4"/>
     <sheet name="pitstop" sheetId="2" r:id="rId5"/>
     <sheet name="lapdelta" sheetId="10" r:id="rId6"/>
-    <sheet name="lapsundercut" sheetId="11" r:id="rId7"/>
+    <sheet name="lapsundercut" sheetId="16" r:id="rId7"/>
     <sheet name="weather" sheetId="14" r:id="rId8"/>
     <sheet name="altitude" sheetId="15" r:id="rId9"/>
-    <sheet name="finalstanding" sheetId="13" r:id="rId10"/>
-    <sheet name="integrated" sheetId="12" r:id="rId11"/>
+    <sheet name="turns" sheetId="18" r:id="rId10"/>
+    <sheet name="finalstanding" sheetId="13" r:id="rId11"/>
+    <sheet name="compoundchange" sheetId="12" r:id="rId12"/>
+    <sheet name="raceclassification" sheetId="19" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,9 +46,10 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -57,16 +60,30 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="157">
   <si>
     <t>Pos.</t>
   </si>
@@ -413,9 +430,6 @@
     <t>no_of_pits</t>
   </si>
   <si>
-    <t>laps_travelled</t>
-  </si>
-  <si>
     <t>tyre_grid</t>
   </si>
   <si>
@@ -463,15 +477,94 @@
   <si>
     <t>delta</t>
   </si>
+  <si>
+    <t>position_after_pit</t>
+  </si>
+  <si>
+    <t>sc</t>
+  </si>
+  <si>
+    <t>turns</t>
+  </si>
+  <si>
+    <t>Nat</t>
+  </si>
+  <si>
+    <t>Laps</t>
+  </si>
+  <si>
+    <t>Interval</t>
+  </si>
+  <si>
+    <t>Kph</t>
+  </si>
+  <si>
+    <t>Best</t>
+  </si>
+  <si>
+    <t>Great Britain</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Monaco</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>1 Lap</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>2 Laps</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>total_time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="mm:ss.000"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss.000"/>
     <numFmt numFmtId="166" formatCode="h:mm:ss.000"/>
+    <numFmt numFmtId="167" formatCode="h\.mm\.ss.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -543,7 +636,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -553,6 +646,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -570,6 +664,65 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>0</v>
+    <v>8</v>
+    <v>0</v>
+    <v>3</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="colOffset" t="i"/>
+    <k n="errorType" t="i"/>
+    <k n="rwOffset" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -872,7 +1025,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,11 +1526,34 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C01758-0CEB-4330-B870-5BE96DFAD435}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26D98304-78C6-4441-B29A-934F8866B9A0}">
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,805 +1756,1996 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9768B7BF-17E8-4A06-86B3-7F23C0B7186B}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <f>MATCH(A2,lapchart!$B$2:$U$2,0)</f>
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A2,finalstanding!B:B,0))</f>
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <f>COUNTIF(pitstop!A:A, A2)</f>
+        <v>2</v>
+      </c>
+      <c r="E2" cm="1">
+        <f t="array" ref="E2">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A2,ROW(pitstop!A:A),""),COLUMNS($E$1:E1))),"")</f>
+        <v>5</v>
+      </c>
+      <c r="F2" cm="1">
+        <f t="array" ref="F2">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A2,ROW(pitstop!A:A),""),COLUMNS($E$1:F1))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A2,ROW(pitstop!A:A),""),COLUMNS($E$1:E1)))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="G2" cm="1">
+        <f t="array" ref="G2">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A2,ROW(pitstop!A:A),""),COLUMNS($E$1:F1))),F2)</f>
+        <v>4</v>
+      </c>
+      <c r="H2" cm="1">
+        <f t="array" ref="H2">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A2,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>11</v>
+      </c>
+      <c r="I2" cm="1">
+        <f t="array" ref="I2">IFERROR(IF(D2=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H2,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A2=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H2),"")</f>
+        <v>31</v>
+      </c>
+      <c r="J2" cm="1">
+        <f t="array" ref="J2">IFERROR(IF(D2=1,0,IF(D2=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H2-I2,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A2=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H2-I2)),"")</f>
+        <v>13</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2:L21" si="0">IFERROR((C2-B2)*-1,"")</f>
+        <v>-4</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ref="M2:M21" si="1">IF(C2=1,25,IF(C2=2,18,IF(C2=3,15,IF(C2=4,12,IF(C2=5,10,IF(C2=6,8,IF(C2=7,6,IF(C2=8,4,IF(C2=9,2,IF(C2=10,1,0))))))))))</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="9">
+        <f>VLOOKUP(A2,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A2,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A2,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A2,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.7103437499999988E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <f>MATCH(A3,lapchart!$B$2:$U$2,0)</f>
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A3,finalstanding!B:B,0))</f>
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <f>COUNTIF(pitstop!A:A, A3)</f>
+        <v>1</v>
+      </c>
+      <c r="E3" cm="1">
+        <f t="array" ref="E3">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A3,ROW(pitstop!A:A),""),COLUMNS($E$1:E2))),"")</f>
+        <v>5</v>
+      </c>
+      <c r="F3" cm="1">
+        <f t="array" ref="F3">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A3,ROW(pitstop!A:A),""),COLUMNS($E$1:F2))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A3,ROW(pitstop!A:A),""),COLUMNS($E$1:E2)))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="G3" cm="1">
+        <f t="array" ref="G3">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A3,ROW(pitstop!A:A),""),COLUMNS($E$1:F2))),F3)</f>
+        <v>3</v>
+      </c>
+      <c r="H3" cm="1">
+        <f t="array" ref="H3">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A3,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>8</v>
+      </c>
+      <c r="I3" cm="1">
+        <f t="array" ref="I3">IFERROR(IF(D3=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H3,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A3=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H3),"")</f>
+        <v>47</v>
+      </c>
+      <c r="J3" cm="1">
+        <f t="array" ref="J3">IFERROR(IF(D3=1,0,IF(D3=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H3-I3,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A3=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H3-I3)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="N3" s="9">
+        <f>VLOOKUP(A3,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A3,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A3,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A3,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.7036793981481477E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <f>MATCH(A4,lapchart!$B$2:$U$2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A4,finalstanding!B:B,0))</f>
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <f>COUNTIF(pitstop!A:A, A4)</f>
+        <v>2</v>
+      </c>
+      <c r="E4" cm="1">
+        <f t="array" ref="E4">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A4,ROW(pitstop!A:A),""),COLUMNS($E$1:E3))),"")</f>
+        <v>5</v>
+      </c>
+      <c r="F4" cm="1">
+        <f t="array" ref="F4">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A4,ROW(pitstop!A:A),""),COLUMNS($E$1:F3))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A4,ROW(pitstop!A:A),""),COLUMNS($E$1:E3)))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="G4" cm="1">
+        <f t="array" ref="G4">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A4,ROW(pitstop!A:A),""),COLUMNS($E$1:F3))),F4)</f>
+        <v>4</v>
+      </c>
+      <c r="H4" cm="1">
+        <f t="array" ref="H4">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A4,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>12</v>
+      </c>
+      <c r="I4" cm="1">
+        <f t="array" ref="I4">IFERROR(IF(D4=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H4,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A4=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H4),"")</f>
+        <v>26</v>
+      </c>
+      <c r="J4" cm="1">
+        <f t="array" ref="J4">IFERROR(IF(D4=1,0,IF(D4=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H4-I4,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A4=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H4-I4)),"")</f>
+        <v>17</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="N4" s="9">
+        <f>VLOOKUP(A4,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A4,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A4,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A4,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.6088796296296298E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>MATCH(A5,lapchart!$B$2:$U$2,0)</f>
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A5,finalstanding!B:B,0))</f>
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <f>COUNTIF(pitstop!A:A, A5)</f>
+        <v>1</v>
+      </c>
+      <c r="E5" cm="1">
+        <f t="array" ref="E5">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A5,ROW(pitstop!A:A),""),COLUMNS($E$1:E4))),"")</f>
+        <v>4</v>
+      </c>
+      <c r="F5" cm="1">
+        <f t="array" ref="F5">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A5,ROW(pitstop!A:A),""),COLUMNS($E$1:F4))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A5,ROW(pitstop!A:A),""),COLUMNS($E$1:E4)))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="G5" cm="1">
+        <f t="array" ref="G5">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A5,ROW(pitstop!A:A),""),COLUMNS($E$1:F4))),F5)</f>
+        <v>3</v>
+      </c>
+      <c r="H5" cm="1">
+        <f t="array" ref="H5">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A5,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>22</v>
+      </c>
+      <c r="I5" cm="1">
+        <f t="array" ref="I5">IFERROR(IF(D5=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H5,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A5=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H5),"")</f>
+        <v>33</v>
+      </c>
+      <c r="J5" cm="1">
+        <f t="array" ref="J5">IFERROR(IF(D5=1,0,IF(D5=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H5-I5,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A5=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H5-I5)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="9">
+        <f>VLOOKUP(A5,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A5,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A5,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A5,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.720480324074074E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>MATCH(A6,lapchart!$B$2:$U$2,0)</f>
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A6,finalstanding!B:B,0))</f>
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <f>COUNTIF(pitstop!A:A, A6)</f>
+        <v>1</v>
+      </c>
+      <c r="E6" cm="1">
+        <f t="array" ref="E6">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A6,ROW(pitstop!A:A),""),COLUMNS($E$1:E5))),"")</f>
+        <v>4</v>
+      </c>
+      <c r="F6" cm="1">
+        <f t="array" ref="F6">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A6,ROW(pitstop!A:A),""),COLUMNS($E$1:F5))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A6,ROW(pitstop!A:A),""),COLUMNS($E$1:E5)))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="G6" cm="1">
+        <f t="array" ref="G6">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A6,ROW(pitstop!A:A),""),COLUMNS($E$1:F5))),F6)</f>
+        <v>3</v>
+      </c>
+      <c r="H6" cm="1">
+        <f t="array" ref="H6">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A6,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>18</v>
+      </c>
+      <c r="I6" cm="1">
+        <f t="array" ref="I6">IFERROR(IF(D6=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H6,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A6=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H6),"")</f>
+        <v>37</v>
+      </c>
+      <c r="J6" cm="1">
+        <f t="array" ref="J6">IFERROR(IF(D6=1,0,IF(D6=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H6-I6,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A6=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H6-I6)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="9">
+        <f>VLOOKUP(A6,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A6,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A6,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A6,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.7597997685185179E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <f>MATCH(A7,lapchart!$B$2:$U$2,0)</f>
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A7,finalstanding!B:B,0))</f>
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <f>COUNTIF(pitstop!A:A, A7)</f>
+        <v>1</v>
+      </c>
+      <c r="E7" cm="1">
+        <f t="array" ref="E7">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A7,ROW(pitstop!A:A),""),COLUMNS($E$1:E6))),"")</f>
+        <v>4</v>
+      </c>
+      <c r="F7" cm="1">
+        <f t="array" ref="F7">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A7,ROW(pitstop!A:A),""),COLUMNS($E$1:F6))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A7,ROW(pitstop!A:A),""),COLUMNS($E$1:E6)))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="G7" cm="1">
+        <f t="array" ref="G7">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A7,ROW(pitstop!A:A),""),COLUMNS($E$1:F6))),F7)</f>
+        <v>3</v>
+      </c>
+      <c r="H7" cm="1">
+        <f t="array" ref="H7">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A7,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>1</v>
+      </c>
+      <c r="I7" cm="1">
+        <f t="array" ref="I7">IFERROR(IF(D7=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H7,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A7=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H7),"")</f>
+        <v>54</v>
+      </c>
+      <c r="J7" cm="1">
+        <f t="array" ref="J7">IFERROR(IF(D7=1,0,IF(D7=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H7-I7,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A7=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H7-I7)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="9">
+        <f>VLOOKUP(A7,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A7,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A7,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A7,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.9641215277777779E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <f>MATCH(A8,lapchart!$B$2:$U$2,0)</f>
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A8,finalstanding!B:B,0))</f>
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <f>COUNTIF(pitstop!A:A, A8)</f>
+        <v>1</v>
+      </c>
+      <c r="E8" cm="1">
+        <f t="array" ref="E8">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A8,ROW(pitstop!A:A),""),COLUMNS($E$1:E7))),"")</f>
+        <v>4</v>
+      </c>
+      <c r="F8" cm="1">
+        <f t="array" ref="F8">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A8,ROW(pitstop!A:A),""),COLUMNS($E$1:F7))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A8,ROW(pitstop!A:A),""),COLUMNS($E$1:E7)))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="G8" cm="1">
+        <f t="array" ref="G8">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A8,ROW(pitstop!A:A),""),COLUMNS($E$1:F7))),F8)</f>
+        <v>3</v>
+      </c>
+      <c r="H8" cm="1">
+        <f t="array" ref="H8">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A8,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>37</v>
+      </c>
+      <c r="I8" cm="1">
+        <f t="array" ref="I8">IFERROR(IF(D8=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H8,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A8=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H8),"")</f>
+        <v>18</v>
+      </c>
+      <c r="J8" cm="1">
+        <f t="array" ref="J8">IFERROR(IF(D8=1,0,IF(D8=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H8-I8,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A8=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H8-I8)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="N8" s="9">
+        <f>VLOOKUP(A8,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A8,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A8,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A8,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.7021041666666656E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <f>MATCH(A9,lapchart!$B$2:$U$2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A9,finalstanding!B:B,0))</f>
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <f>COUNTIF(pitstop!A:A, A9)</f>
+        <v>2</v>
+      </c>
+      <c r="E9" cm="1">
+        <f t="array" ref="E9">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A9,ROW(pitstop!A:A),""),COLUMNS($E$1:E8))),"")</f>
+        <v>4</v>
+      </c>
+      <c r="F9" cm="1">
+        <f t="array" ref="F9">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A9,ROW(pitstop!A:A),""),COLUMNS($E$1:F8))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A9,ROW(pitstop!A:A),""),COLUMNS($E$1:E8)))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="G9" cm="1">
+        <f t="array" ref="G9">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A9,ROW(pitstop!A:A),""),COLUMNS($E$1:F8))),F9)</f>
+        <v>5</v>
+      </c>
+      <c r="H9" cm="1">
+        <f t="array" ref="H9">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A9,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>12</v>
+      </c>
+      <c r="I9" cm="1">
+        <f t="array" ref="I9">IFERROR(IF(D9=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H9,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A9=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H9),"")</f>
+        <v>26</v>
+      </c>
+      <c r="J9" cm="1">
+        <f t="array" ref="J9">IFERROR(IF(D9=1,0,IF(D9=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H9-I9,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A9=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H9-I9)),"")</f>
+        <v>17</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="N9" s="9">
+        <f>VLOOKUP(A9,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A9,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A9,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A9,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.584664351851853E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <f>MATCH(A10,lapchart!$B$2:$U$2,0)</f>
+        <v>12</v>
+      </c>
+      <c r="C10" t="str">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A10,finalstanding!B:B,0))</f>
+        <v>DNF</v>
+      </c>
+      <c r="D10">
+        <f>COUNTIF(pitstop!A:A, A10)</f>
+        <v>2</v>
+      </c>
+      <c r="E10" cm="1">
+        <f t="array" ref="E10">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A10,ROW(pitstop!A:A),""),COLUMNS($E$1:E9))),"")</f>
+        <v>4</v>
+      </c>
+      <c r="F10" cm="1">
+        <f t="array" ref="F10">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A10,ROW(pitstop!A:A),""),COLUMNS($E$1:F9))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A10,ROW(pitstop!A:A),""),COLUMNS($E$1:E9)))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="G10" cm="1">
+        <f t="array" ref="G10">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A10,ROW(pitstop!A:A),""),COLUMNS($E$1:F9))),F10)</f>
+        <v>5</v>
+      </c>
+      <c r="H10" cm="1">
+        <f t="array" ref="H10">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A10,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>5</v>
+      </c>
+      <c r="I10" cm="1">
+        <f t="array" ref="I10">IFERROR(IF(D10=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H10,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A10=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H10),"")</f>
+        <v>18</v>
+      </c>
+      <c r="J10" cm="1">
+        <f t="array" ref="J10">IFERROR(IF(D10=1,0,IF(D10=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H10-I10,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A10=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H10-I10)),"")</f>
+        <v>32</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="9">
+        <f>VLOOKUP(A10,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A10,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A10,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A10,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>5.5705196759259258E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <f>MATCH(A11,lapchart!$B$2:$U$2,0)</f>
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A11,finalstanding!B:B,0))</f>
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <f>COUNTIF(pitstop!A:A, A11)</f>
+        <v>1</v>
+      </c>
+      <c r="E11" cm="1">
+        <f t="array" ref="E11">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A11,ROW(pitstop!A:A),""),COLUMNS($E$1:E10))),"")</f>
+        <v>4</v>
+      </c>
+      <c r="F11" cm="1">
+        <f t="array" ref="F11">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A11,ROW(pitstop!A:A),""),COLUMNS($E$1:F10))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A11,ROW(pitstop!A:A),""),COLUMNS($E$1:E10)))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="G11" cm="1">
+        <f t="array" ref="G11">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A11,ROW(pitstop!A:A),""),COLUMNS($E$1:F10))),F11)</f>
+        <v>3</v>
+      </c>
+      <c r="H11" cm="1">
+        <f t="array" ref="H11">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A11,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>20</v>
+      </c>
+      <c r="I11" cm="1">
+        <f t="array" ref="I11">IFERROR(IF(D11=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H11,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A11=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H11),"")</f>
+        <v>35</v>
+      </c>
+      <c r="J11" cm="1">
+        <f t="array" ref="J11">IFERROR(IF(D11=1,0,IF(D11=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H11-I11,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A11=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H11-I11)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="9">
+        <f>VLOOKUP(A11,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A11,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A11,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A11,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.7378414351851851E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <f>MATCH(A12,lapchart!$B$2:$U$2,0)</f>
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A12,finalstanding!B:B,0))</f>
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <f>COUNTIF(pitstop!A:A, A12)</f>
+        <v>1</v>
+      </c>
+      <c r="E12" cm="1">
+        <f t="array" ref="E12">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A12,ROW(pitstop!A:A),""),COLUMNS($E$1:E11))),"")</f>
+        <v>4</v>
+      </c>
+      <c r="F12" cm="1">
+        <f t="array" ref="F12">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A12,ROW(pitstop!A:A),""),COLUMNS($E$1:F11))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A12,ROW(pitstop!A:A),""),COLUMNS($E$1:E11)))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="G12" cm="1">
+        <f t="array" ref="G12">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A12,ROW(pitstop!A:A),""),COLUMNS($E$1:F11))),F12)</f>
+        <v>3</v>
+      </c>
+      <c r="H12" cm="1">
+        <f t="array" ref="H12">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A12,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>13</v>
+      </c>
+      <c r="I12" cm="1">
+        <f t="array" ref="I12">IFERROR(IF(D12=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H12,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A12=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H12),"")</f>
+        <v>42</v>
+      </c>
+      <c r="J12" cm="1">
+        <f t="array" ref="J12">IFERROR(IF(D12=1,0,IF(D12=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H12-I12,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A12=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H12-I12)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="N12" s="9">
+        <f>VLOOKUP(A12,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A12,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A12,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A12,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.6144907407407402E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <f>MATCH(A13,lapchart!$B$2:$U$2,0)</f>
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A13,finalstanding!B:B,0))</f>
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <f>COUNTIF(pitstop!A:A, A13)</f>
+        <v>1</v>
+      </c>
+      <c r="E13" cm="1">
+        <f t="array" ref="E13">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A13,ROW(pitstop!A:A),""),COLUMNS($E$1:E12))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="F13" cm="1">
+        <f t="array" ref="F13">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A13,ROW(pitstop!A:A),""),COLUMNS($E$1:F12))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A13,ROW(pitstop!A:A),""),COLUMNS($E$1:E12)))),"")</f>
+        <v>4</v>
+      </c>
+      <c r="G13" cm="1">
+        <f t="array" ref="G13">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A13,ROW(pitstop!A:A),""),COLUMNS($E$1:F12))),F13)</f>
+        <v>4</v>
+      </c>
+      <c r="H13" cm="1">
+        <f t="array" ref="H13">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A13,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>40</v>
+      </c>
+      <c r="I13" cm="1">
+        <f t="array" ref="I13">IFERROR(IF(D13=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H13,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A13=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H13),"")</f>
+        <v>15</v>
+      </c>
+      <c r="J13" cm="1">
+        <f t="array" ref="J13">IFERROR(IF(D13=1,0,IF(D13=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H13-I13,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A13=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H13-I13)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N13" s="9">
+        <f>VLOOKUP(A13,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A13,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A13,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A13,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.7051342592592586E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <f>MATCH(A14,lapchart!$B$2:$U$2,0)</f>
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A14,finalstanding!B:B,0))</f>
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <f>COUNTIF(pitstop!A:A, A14)</f>
+        <v>1</v>
+      </c>
+      <c r="E14" cm="1">
+        <f t="array" ref="E14">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A14,ROW(pitstop!A:A),""),COLUMNS($E$1:E13))),"")</f>
+        <v>5</v>
+      </c>
+      <c r="F14" cm="1">
+        <f t="array" ref="F14">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A14,ROW(pitstop!A:A),""),COLUMNS($E$1:F13))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A14,ROW(pitstop!A:A),""),COLUMNS($E$1:E13)))),"")</f>
+        <v>4</v>
+      </c>
+      <c r="G14" cm="1">
+        <f t="array" ref="G14">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A14,ROW(pitstop!A:A),""),COLUMNS($E$1:F13))),F14)</f>
+        <v>4</v>
+      </c>
+      <c r="H14" cm="1">
+        <f t="array" ref="H14">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A14,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>18</v>
+      </c>
+      <c r="I14" cm="1">
+        <f t="array" ref="I14">IFERROR(IF(D14=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H14,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A14=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H14),"")</f>
+        <v>37</v>
+      </c>
+      <c r="J14" cm="1">
+        <f t="array" ref="J14">IFERROR(IF(D14=1,0,IF(D14=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H14-I14,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A14=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H14-I14)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="9">
+        <f>VLOOKUP(A14,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A14,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A14,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A14,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.7119143518518512E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>33</v>
+      </c>
+      <c r="B15">
+        <f>MATCH(A15,lapchart!$B$2:$U$2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A15,finalstanding!B:B,0))</f>
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f>COUNTIF(pitstop!A:A, A15)</f>
+        <v>1</v>
+      </c>
+      <c r="E15" cm="1">
+        <f t="array" ref="E15">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A15,ROW(pitstop!A:A),""),COLUMNS($E$1:E14))),"")</f>
+        <v>4</v>
+      </c>
+      <c r="F15" cm="1">
+        <f t="array" ref="F15">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A15,ROW(pitstop!A:A),""),COLUMNS($E$1:F14))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A15,ROW(pitstop!A:A),""),COLUMNS($E$1:E14)))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="G15" cm="1">
+        <f t="array" ref="G15">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A15,ROW(pitstop!A:A),""),COLUMNS($E$1:F14))),F15)</f>
+        <v>3</v>
+      </c>
+      <c r="H15" cm="1">
+        <f t="array" ref="H15">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A15,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>25</v>
+      </c>
+      <c r="I15" cm="1">
+        <f t="array" ref="I15">IFERROR(IF(D15=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H15,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A15=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H15),"")</f>
+        <v>30</v>
+      </c>
+      <c r="J15" cm="1">
+        <f t="array" ref="J15">IFERROR(IF(D15=1,0,IF(D15=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H15-I15,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A15=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H15-I15)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="N15" s="9">
+        <f>VLOOKUP(A15,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A15,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A15,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A15,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.5538043981481484E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>44</v>
+      </c>
+      <c r="B16">
+        <f>MATCH(A16,lapchart!$B$2:$U$2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A16,finalstanding!B:B,0))</f>
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <f>COUNTIF(pitstop!A:A, A16)</f>
+        <v>1</v>
+      </c>
+      <c r="E16" cm="1">
+        <f t="array" ref="E16">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A16,ROW(pitstop!A:A),""),COLUMNS($E$1:E15))),"")</f>
+        <v>4</v>
+      </c>
+      <c r="F16" cm="1">
+        <f t="array" ref="F16">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A16,ROW(pitstop!A:A),""),COLUMNS($E$1:F15))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A16,ROW(pitstop!A:A),""),COLUMNS($E$1:E15)))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="G16" cm="1">
+        <f t="array" ref="G16">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A16,ROW(pitstop!A:A),""),COLUMNS($E$1:F15))),F16)</f>
+        <v>3</v>
+      </c>
+      <c r="H16" cm="1">
+        <f t="array" ref="H16">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A16,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>26</v>
+      </c>
+      <c r="I16" cm="1">
+        <f t="array" ref="I16">IFERROR(IF(D16=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H16,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A16=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H16),"")</f>
+        <v>29</v>
+      </c>
+      <c r="J16" cm="1">
+        <f t="array" ref="J16">IFERROR(IF(D16=1,0,IF(D16=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H16-I16,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A16=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H16-I16)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="N16" s="9">
+        <f>VLOOKUP(A16,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A16,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A16,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A16,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.5343923611111118E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>55</v>
+      </c>
+      <c r="B17">
+        <f>MATCH(A17,lapchart!$B$2:$U$2,0)</f>
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A17,finalstanding!B:B,0))</f>
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <f>COUNTIF(pitstop!A:A, A17)</f>
+        <v>2</v>
+      </c>
+      <c r="E17" cm="1">
+        <f t="array" ref="E17">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A17,ROW(pitstop!A:A),""),COLUMNS($E$1:E16))),"")</f>
+        <v>5</v>
+      </c>
+      <c r="F17" cm="1">
+        <f t="array" ref="F17">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A17,ROW(pitstop!A:A),""),COLUMNS($E$1:F16))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A17,ROW(pitstop!A:A),""),COLUMNS($E$1:E16)))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="G17" cm="1">
+        <f t="array" ref="G17">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A17,ROW(pitstop!A:A),""),COLUMNS($E$1:F16))),F17)</f>
+        <v>4</v>
+      </c>
+      <c r="H17" cm="1">
+        <f t="array" ref="H17">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A17,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>12</v>
+      </c>
+      <c r="I17" cm="1">
+        <f t="array" ref="I17">IFERROR(IF(D17=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H17,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A17=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H17),"")</f>
+        <v>29</v>
+      </c>
+      <c r="J17" cm="1">
+        <f t="array" ref="J17">IFERROR(IF(D17=1,0,IF(D17=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H17-I17,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A17=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H17-I17)),"")</f>
+        <v>14</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N17" s="9">
+        <f>VLOOKUP(A17,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A17,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A17,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A17,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.7093009259259262E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>63</v>
+      </c>
+      <c r="B18">
+        <f>MATCH(A18,lapchart!$B$2:$U$2,0)</f>
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A18,finalstanding!B:B,0))</f>
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <f>COUNTIF(pitstop!A:A, A18)</f>
+        <v>1</v>
+      </c>
+      <c r="E18" cm="1">
+        <f t="array" ref="E18">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A18,ROW(pitstop!A:A),""),COLUMNS($E$1:E17))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="F18" cm="1">
+        <f t="array" ref="F18">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A18,ROW(pitstop!A:A),""),COLUMNS($E$1:F17))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A18,ROW(pitstop!A:A),""),COLUMNS($E$1:E17)))),"")</f>
+        <v>4</v>
+      </c>
+      <c r="G18" cm="1">
+        <f t="array" ref="G18">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A18,ROW(pitstop!A:A),""),COLUMNS($E$1:F17))),F18)</f>
+        <v>4</v>
+      </c>
+      <c r="H18" cm="1">
+        <f t="array" ref="H18">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A18,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>32</v>
+      </c>
+      <c r="I18" cm="1">
+        <f t="array" ref="I18">IFERROR(IF(D18=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H18,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A18=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H18),"")</f>
+        <v>23</v>
+      </c>
+      <c r="J18" cm="1">
+        <f t="array" ref="J18">IFERROR(IF(D18=1,0,IF(D18=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H18-I18,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A18=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H18-I18)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="9">
+        <f>VLOOKUP(A18,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A18,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A18,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A18,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.7864571759259251E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>77</v>
+      </c>
+      <c r="B19">
+        <f>MATCH(A19,lapchart!$B$2:$U$2,0)</f>
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A19,finalstanding!B:B,0))</f>
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <f>COUNTIF(pitstop!A:A, A19)</f>
+        <v>1</v>
+      </c>
+      <c r="E19" cm="1">
+        <f t="array" ref="E19">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A19,ROW(pitstop!A:A),""),COLUMNS($E$1:E18))),"")</f>
+        <v>4</v>
+      </c>
+      <c r="F19" cm="1">
+        <f t="array" ref="F19">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A19,ROW(pitstop!A:A),""),COLUMNS($E$1:F18))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A19,ROW(pitstop!A:A),""),COLUMNS($E$1:E18)))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="G19" cm="1">
+        <f t="array" ref="G19">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A19,ROW(pitstop!A:A),""),COLUMNS($E$1:F18))),F19)</f>
+        <v>3</v>
+      </c>
+      <c r="H19" cm="1">
+        <f t="array" ref="H19">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A19,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>29</v>
+      </c>
+      <c r="I19" cm="1">
+        <f t="array" ref="I19">IFERROR(IF(D19=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H19,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A19=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H19),"")</f>
+        <v>26</v>
+      </c>
+      <c r="J19" cm="1">
+        <f t="array" ref="J19">IFERROR(IF(D19=1,0,IF(D19=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H19-I19,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A19=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H19-I19)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="N19" s="9">
+        <f>VLOOKUP(A19,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A19,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A19,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A19,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.5857569444444444E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>88</v>
+      </c>
+      <c r="B20">
+        <f>MATCH(A20,lapchart!$B$2:$U$2,0)</f>
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A20,finalstanding!B:B,0))</f>
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <f>COUNTIF(pitstop!A:A, A20)</f>
+        <v>1</v>
+      </c>
+      <c r="E20" cm="1">
+        <f t="array" ref="E20">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A20,ROW(pitstop!A:A),""),COLUMNS($E$1:E19))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="F20" cm="1">
+        <f t="array" ref="F20">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A20,ROW(pitstop!A:A),""),COLUMNS($E$1:F19))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A20,ROW(pitstop!A:A),""),COLUMNS($E$1:E19)))),"")</f>
+        <v>4</v>
+      </c>
+      <c r="G20" cm="1">
+        <f t="array" ref="G20">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A20,ROW(pitstop!A:A),""),COLUMNS($E$1:F19))),F20)</f>
+        <v>4</v>
+      </c>
+      <c r="H20" cm="1">
+        <f t="array" ref="H20">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A20,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>24</v>
+      </c>
+      <c r="I20" cm="1">
+        <f t="array" ref="I20">IFERROR(IF(D20=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H20,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A20=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H20),"")</f>
+        <v>31</v>
+      </c>
+      <c r="J20" cm="1">
+        <f t="array" ref="J20">IFERROR(IF(D20=1,0,IF(D20=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H20-I20,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A20=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H20-I20)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="9">
+        <f>VLOOKUP(A20,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A20,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A20,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A20,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.9785567129629633E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>99</v>
+      </c>
+      <c r="B21">
+        <f>MATCH(A21,lapchart!$B$2:$U$2,0)</f>
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <f>INDEX(finalstanding!A:A,MATCH(compoundchange!A21,finalstanding!B:B,0))</f>
+        <v>16</v>
+      </c>
+      <c r="D21">
+        <f>COUNTIF(pitstop!A:A, A21)</f>
+        <v>2</v>
+      </c>
+      <c r="E21" cm="1">
+        <f t="array" ref="E21">IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A21,ROW(pitstop!A:A),""),COLUMNS($E$1:E20))),"")</f>
+        <v>5</v>
+      </c>
+      <c r="F21" cm="1">
+        <f t="array" ref="F21">IFERROR(IFERROR(INDEX(pitstop!H:H,SMALL(IF(pitstop!A:A=A21,ROW(pitstop!A:A),""),COLUMNS($E$1:F20))),INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A21,ROW(pitstop!A:A),""),COLUMNS($E$1:E20)))),"")</f>
+        <v>3</v>
+      </c>
+      <c r="G21" cm="1">
+        <f t="array" ref="G21">IFERROR(INDEX(pitstop!I:I,SMALL(IF(pitstop!A:A=A21,ROW(pitstop!A:A),""),COLUMNS($E$1:F20))),F21)</f>
+        <v>4</v>
+      </c>
+      <c r="H21" cm="1">
+        <f t="array" ref="H21">IFERROR(INDEX(pitstop!D:D,SMALL(IF(pitstop!A:A=A21,ROW(pitstop!A:A),""),1)),"")</f>
+        <v>8</v>
+      </c>
+      <c r="I21" cm="1">
+        <f t="array" ref="I21">IFERROR(IF(D21=1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H21,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A21=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H21),"")</f>
+        <v>18</v>
+      </c>
+      <c r="J21" cm="1">
+        <f t="array" ref="J21">IFERROR(IF(D21=1,0,IF(D21=2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-H21-I21,INDEX(pitstop!$D$2:$D$100,SMALL(IF(compoundchange!$A21=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1))-H21-I21)),"")</f>
+        <v>29</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="9">
+        <f>VLOOKUP(A21,raceclassification!B:G,6,FALSE)+IF(ISNUMBER(SEARCH("Lap",VLOOKUP(A21,raceclassification!B:H,7,FALSE))),IF(VLOOKUP(A21,raceclassification!B:H,7,FALSE)="1 Lap","0:02",IF(VLOOKUP(A21,raceclassification!B:H,7,FALSE)="2 Lap","0:04","0:06")),0)</f>
+        <v>6.7737060185185174E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2BAA5C-15AA-4BA7-A555-83C5C3DD6136}">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>121</v>
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <f>MATCH(A2,lapchart!B2:U2,0)</f>
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A2,finalstanding!B:B,0))</f>
-        <v>11</v>
-      </c>
-      <c r="D2">
-        <f>IFERROR(C2-B2,"DNF")</f>
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <f>IF(C2=1,25,IF(C2=2,18,IF(C2=3,15,IF(C2=4,12,IF(C2=5,10,IF(C2=6,8,IF(C2=7,6,IF(C2=8,4,IF(C2=9,2,IF(C2=10,1,0))))))))))</f>
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
       </c>
       <c r="F2">
-        <f>COUNTIF(pitstop!A:A, A2)</f>
-        <v>2</v>
-      </c>
-      <c r="J2" cm="1">
-        <f t="array" ref="J2">IF(F2&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A2=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>11</v>
-      </c>
-      <c r="K2" cm="1">
-        <f t="array" ref="K2">IF(F2&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J2,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A2=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>31</v>
-      </c>
-      <c r="L2" cm="1">
-        <f t="array" ref="L2">IF(F2&lt;3,IF(F2=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K2),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A2=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v>24</v>
+        <v>55</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6.5343923611111118E-2</v>
+      </c>
+      <c r="J2">
+        <v>194.71</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1.1491087962962963E-3</v>
+      </c>
+      <c r="L2">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <f>MATCH(A3,lapchart!B3:U3,0)</f>
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A3,finalstanding!B:B,0))</f>
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D21" si="0">IFERROR(C3-B3,"DNF")</f>
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E21" si="1">IF(C3=1,25,IF(C3=2,18,IF(C3=3,15,IF(C3=4,12,IF(C3=5,10,IF(C3=6,8,IF(C3=7,6,IF(C3=8,4,IF(C3=9,2,IF(C3=10,1,0))))))))))</f>
-        <v>4</v>
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" t="s">
+        <v>73</v>
       </c>
       <c r="F3">
-        <f>COUNTIF(pitstop!A:A, A3)</f>
-        <v>1</v>
-      </c>
-      <c r="J3" cm="1">
-        <f t="array" ref="J3">IF(F3&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A3=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>8</v>
-      </c>
-      <c r="K3" cm="1">
-        <f t="array" ref="K3">IF(F3&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J3,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A3=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>47</v>
-      </c>
-      <c r="L3" t="str" cm="1">
-        <f t="array" ref="L3">IF(F3&lt;3,IF(F3=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K3),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A3=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v/>
+        <v>55</v>
+      </c>
+      <c r="G3" s="1">
+        <v>6.5538043981481484E-2</v>
+      </c>
+      <c r="H3">
+        <v>16.771999999999998</v>
+      </c>
+      <c r="I3">
+        <v>16.771999999999998</v>
+      </c>
+      <c r="J3">
+        <v>194.13300000000001</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1.1703587962962963E-3</v>
+      </c>
+      <c r="L3">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <f>MATCH(A4,lapchart!B4:U4,0)</f>
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A4,finalstanding!B:B,0))</f>
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" t="s">
+        <v>70</v>
       </c>
       <c r="F4">
-        <f>COUNTIF(pitstop!A:A, A4)</f>
-        <v>2</v>
-      </c>
-      <c r="J4" cm="1">
-        <f t="array" ref="J4">IF(F4&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A4=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>12</v>
-      </c>
-      <c r="K4" cm="1">
-        <f t="array" ref="K4">IF(F4&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J4,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A4=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>26</v>
-      </c>
-      <c r="L4" cm="1">
-        <f t="array" ref="L4">IF(F4&lt;3,IF(F4=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K4),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A4=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v>29</v>
+        <v>55</v>
+      </c>
+      <c r="G4" s="1">
+        <v>6.584664351851853E-2</v>
+      </c>
+      <c r="H4">
+        <v>43.435000000000002</v>
+      </c>
+      <c r="I4">
+        <v>26.663</v>
+      </c>
+      <c r="J4">
+        <v>193.22300000000001</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1.1625231481481482E-3</v>
+      </c>
+      <c r="L4">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <f>MATCH(A5,lapchart!B5:U5,0)</f>
-        <v>15</v>
-      </c>
-      <c r="C5">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A5,finalstanding!B:B,0))</f>
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
       </c>
       <c r="F5">
-        <f>COUNTIF(pitstop!A:A, A5)</f>
-        <v>1</v>
-      </c>
-      <c r="J5" cm="1">
-        <f t="array" ref="J5">IF(F5&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A5=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>22</v>
-      </c>
-      <c r="K5" cm="1">
-        <f t="array" ref="K5">IF(F5&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J5,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A5=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>33</v>
-      </c>
-      <c r="L5" t="str" cm="1">
-        <f t="array" ref="L5">IF(F5&lt;3,IF(F5=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K5),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A5=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v/>
+        <v>55</v>
+      </c>
+      <c r="G5" s="1">
+        <v>6.5857569444444444E-2</v>
+      </c>
+      <c r="H5">
+        <v>44.378999999999998</v>
+      </c>
+      <c r="I5">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="J5">
+        <v>193.191</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1.1541087962962963E-3</v>
+      </c>
+      <c r="L5">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <f>MATCH(A6,lapchart!B6:U6,0)</f>
-        <v>17</v>
-      </c>
-      <c r="C6">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A6,finalstanding!B:B,0))</f>
-        <v>15</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" t="s">
+        <v>70</v>
       </c>
       <c r="F6">
-        <f>COUNTIF(pitstop!A:A, A6)</f>
-        <v>1</v>
-      </c>
-      <c r="J6" cm="1">
-        <f t="array" ref="J6">IF(F6&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A6=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>18</v>
-      </c>
-      <c r="K6" cm="1">
-        <f t="array" ref="K6">IF(F6&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J6,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A6=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>37</v>
-      </c>
-      <c r="L6" t="str" cm="1">
-        <f t="array" ref="L6">IF(F6&lt;3,IF(F6=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K6),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A6=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v/>
+        <v>55</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6.6088796296296298E-2</v>
+      </c>
+      <c r="H6" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I6">
+        <v>19.978000000000002</v>
+      </c>
+      <c r="J6">
+        <v>192.51499999999999</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1.158888888888889E-3</v>
+      </c>
+      <c r="L6">
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <f>MATCH(A7,lapchart!B7:U7,0)</f>
-        <v>20</v>
-      </c>
-      <c r="C7">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A7,finalstanding!B:B,0))</f>
-        <v>18</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7">
+        <v>55</v>
+      </c>
+      <c r="G7" s="1">
+        <v>6.6144907407407402E-2</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
-      <c r="F7">
-        <f>COUNTIF(pitstop!A:A, A7)</f>
-        <v>1</v>
-      </c>
-      <c r="J7" cm="1">
-        <f t="array" ref="J7">IF(F7&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A7=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>1</v>
-      </c>
-      <c r="K7" cm="1">
-        <f t="array" ref="K7">IF(F7&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J7,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A7=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>54</v>
-      </c>
-      <c r="L7" t="str" cm="1">
-        <f t="array" ref="L7">IF(F7&lt;3,IF(F7=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K7),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A7=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v/>
+      <c r="I7">
+        <v>4.8479999999999999</v>
+      </c>
+      <c r="J7">
+        <v>192.352</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1.1830902777777779E-3</v>
+      </c>
+      <c r="L7">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>11</v>
       </c>
-      <c r="B8">
-        <f>MATCH(A8,lapchart!B8:U8,0)</f>
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A8,finalstanding!B:B,0))</f>
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
-        <v>6</v>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" t="s">
+        <v>83</v>
       </c>
       <c r="F8">
-        <f>COUNTIF(pitstop!A:A, A8)</f>
-        <v>1</v>
-      </c>
-      <c r="J8" cm="1">
-        <f t="array" ref="J8">IF(F8&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A8=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>37</v>
-      </c>
-      <c r="K8" cm="1">
-        <f t="array" ref="K8">IF(F8&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J8,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A8=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>18</v>
-      </c>
-      <c r="L8" t="str" cm="1">
-        <f t="array" ref="L8">IF(F8&lt;3,IF(F8=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K8),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A8=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v/>
+        <v>54</v>
+      </c>
+      <c r="G8" s="1">
+        <v>6.5632152777777772E-2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I8" t="s">
+        <v>146</v>
+      </c>
+      <c r="J8">
+        <v>190.32900000000001</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1.1879513888888888E-3</v>
+      </c>
+      <c r="L8">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <f>MATCH(A9,lapchart!B9:U9,0)</f>
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A9,finalstanding!B:B,0))</f>
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>15</v>
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" t="s">
+        <v>77</v>
       </c>
       <c r="F9">
-        <f>COUNTIF(pitstop!A:A, A9)</f>
-        <v>2</v>
-      </c>
-      <c r="J9" cm="1">
-        <f t="array" ref="J9">IF(F9&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A9=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>12</v>
-      </c>
-      <c r="K9" cm="1">
-        <f t="array" ref="K9">IF(F9&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J9,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A9=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>26</v>
-      </c>
-      <c r="L9" cm="1">
-        <f t="array" ref="L9">IF(F9&lt;3,IF(F9=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K9),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A9=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v>29</v>
+        <v>54</v>
+      </c>
+      <c r="G9" s="1">
+        <v>6.5647905092592593E-2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>146</v>
+      </c>
+      <c r="I9">
+        <v>1.361</v>
+      </c>
+      <c r="J9">
+        <v>190.28299999999999</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1.1924305555555557E-3</v>
+      </c>
+      <c r="L9">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <f>MATCH(A10,lapchart!B10:U10,0)</f>
-        <v>19</v>
-      </c>
-      <c r="C10" t="str">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A10,finalstanding!B:B,0))</f>
-        <v>DNF</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>DNF</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" t="s">
+        <v>80</v>
       </c>
       <c r="F10">
-        <f>COUNTIF(pitstop!A:A, A10)</f>
-        <v>2</v>
-      </c>
-      <c r="J10" cm="1">
-        <f t="array" ref="J10">IF(F10&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A10=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>5</v>
-      </c>
-      <c r="K10" cm="1">
-        <f t="array" ref="K10">IF(F10&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J10,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A10=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>18</v>
-      </c>
-      <c r="L10" cm="1">
-        <f t="array" ref="L10">IF(F10&lt;3,IF(F10=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K10),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A10=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v>37</v>
+        <v>54</v>
+      </c>
+      <c r="G10" s="1">
+        <v>6.5662453703703702E-2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>146</v>
+      </c>
+      <c r="I10">
+        <v>1.2569999999999999</v>
+      </c>
+      <c r="J10">
+        <v>190.24100000000001</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1.1831249999999999E-3</v>
+      </c>
+      <c r="L10">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <f>MATCH(A11,lapchart!B11:U11,0)</f>
-        <v>11</v>
-      </c>
-      <c r="C11">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A11,finalstanding!B:B,0))</f>
-        <v>14</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" t="s">
+        <v>77</v>
       </c>
       <c r="F11">
-        <f>COUNTIF(pitstop!A:A, A11)</f>
-        <v>1</v>
-      </c>
-      <c r="J11" cm="1">
-        <f t="array" ref="J11">IF(F11&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A11=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>20</v>
-      </c>
-      <c r="K11" cm="1">
-        <f t="array" ref="K11">IF(F11&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J11,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A11=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>35</v>
-      </c>
-      <c r="L11" t="str" cm="1">
-        <f t="array" ref="L11">IF(F11&lt;3,IF(F11=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K11),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A11=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v/>
+        <v>54</v>
+      </c>
+      <c r="G11" s="1">
+        <v>6.5704120370370378E-2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I11">
+        <v>3.6</v>
+      </c>
+      <c r="J11">
+        <v>190.12</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1.1723842592592591E-3</v>
+      </c>
+      <c r="L11">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <f>MATCH(A12,lapchart!B12:U12,0)</f>
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A12,finalstanding!B:B,0))</f>
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" t="s">
+        <v>149</v>
+      </c>
+      <c r="E12" t="s">
+        <v>75</v>
       </c>
       <c r="F12">
-        <f>COUNTIF(pitstop!A:A, A12)</f>
-        <v>1</v>
-      </c>
-      <c r="J12" cm="1">
-        <f t="array" ref="J12">IF(F12&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A12=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>13</v>
-      </c>
-      <c r="K12" cm="1">
-        <f t="array" ref="K12">IF(F12&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J12,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A12=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>42</v>
-      </c>
-      <c r="L12" t="str" cm="1">
-        <f t="array" ref="L12">IF(F12&lt;3,IF(F12=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K12),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A12=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v/>
+        <v>54</v>
+      </c>
+      <c r="G12" s="1">
+        <v>6.5714548611111104E-2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>146</v>
+      </c>
+      <c r="I12">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="J12">
+        <v>190.09</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1.1711805555555557E-3</v>
+      </c>
+      <c r="L12">
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <f>MATCH(A13,lapchart!B13:U13,0)</f>
-        <v>13</v>
-      </c>
-      <c r="C13">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A13,finalstanding!B:B,0))</f>
-        <v>9</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
       </c>
       <c r="F13">
-        <f>COUNTIF(pitstop!A:A, A13)</f>
-        <v>1</v>
-      </c>
-      <c r="J13" cm="1">
-        <f t="array" ref="J13">IF(F13&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A13=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>40</v>
-      </c>
-      <c r="K13" cm="1">
-        <f t="array" ref="K13">IF(F13&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J13,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A13=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>15</v>
-      </c>
-      <c r="L13" t="str" cm="1">
-        <f t="array" ref="L13">IF(F13&lt;3,IF(F13=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K13),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A13=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v/>
+        <v>54</v>
+      </c>
+      <c r="G13" s="1">
+        <v>6.5730254629629628E-2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>146</v>
+      </c>
+      <c r="I13">
+        <v>1.357</v>
+      </c>
+      <c r="J13">
+        <v>190.04499999999999</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1.1953009259259258E-3</v>
+      </c>
+      <c r="L13">
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <f>MATCH(A14,lapchart!B14:U14,0)</f>
-        <v>6</v>
-      </c>
-      <c r="C14">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A14,finalstanding!B:B,0))</f>
-        <v>12</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" t="s">
+        <v>142</v>
+      </c>
+      <c r="E14" t="s">
+        <v>88</v>
       </c>
       <c r="F14">
-        <f>COUNTIF(pitstop!A:A, A14)</f>
-        <v>1</v>
-      </c>
-      <c r="J14" cm="1">
-        <f t="array" ref="J14">IF(F14&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A14=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>18</v>
-      </c>
-      <c r="K14" cm="1">
-        <f t="array" ref="K14">IF(F14&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J14,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A14=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>37</v>
-      </c>
-      <c r="L14" t="str" cm="1">
-        <f t="array" ref="L14">IF(F14&lt;3,IF(F14=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K14),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A14=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v/>
+        <v>54</v>
+      </c>
+      <c r="G14" s="1">
+        <v>6.5815914351851856E-2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>146</v>
+      </c>
+      <c r="I14">
+        <v>7.4009999999999998</v>
+      </c>
+      <c r="J14">
+        <v>189.797</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1.1937731481481482E-3</v>
+      </c>
+      <c r="L14">
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <f>MATCH(A15,lapchart!B15:U15,0)</f>
-        <v>2</v>
-      </c>
-      <c r="C15">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A15,finalstanding!B:B,0))</f>
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" t="s">
+        <v>150</v>
+      </c>
+      <c r="E15" t="s">
+        <v>93</v>
       </c>
       <c r="F15">
-        <f>COUNTIF(pitstop!A:A, A15)</f>
-        <v>1</v>
-      </c>
-      <c r="J15" cm="1">
-        <f t="array" ref="J15">IF(F15&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A15=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>25</v>
-      </c>
-      <c r="K15" cm="1">
-        <f t="array" ref="K15">IF(F15&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J15,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A15=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>30</v>
-      </c>
-      <c r="L15" t="str" cm="1">
-        <f t="array" ref="L15">IF(F15&lt;3,IF(F15=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K15),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A15=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v/>
+        <v>54</v>
+      </c>
+      <c r="G15" s="1">
+        <v>6.5989525462962967E-2</v>
+      </c>
+      <c r="H15" t="s">
+        <v>146</v>
+      </c>
+      <c r="I15">
+        <v>15</v>
+      </c>
+      <c r="J15">
+        <v>189.298</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1.2012731481481481E-3</v>
+      </c>
+      <c r="L15">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <f>MATCH(A16,lapchart!B16:U16,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A16,finalstanding!B:B,0))</f>
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
-        <v>25</v>
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" t="s">
+        <v>151</v>
+      </c>
+      <c r="E16" t="s">
+        <v>93</v>
       </c>
       <c r="F16">
-        <f>COUNTIF(pitstop!A:A, A16)</f>
-        <v>1</v>
-      </c>
-      <c r="J16" cm="1">
-        <f t="array" ref="J16">IF(F16&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A16=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>26</v>
-      </c>
-      <c r="K16" cm="1">
-        <f t="array" ref="K16">IF(F16&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J16,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A16=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>29</v>
-      </c>
-      <c r="L16" t="str" cm="1">
-        <f t="array" ref="L16">IF(F16&lt;3,IF(F16=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K16),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A16=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v/>
+        <v>54</v>
+      </c>
+      <c r="G16" s="1">
+        <v>6.6209108796296295E-2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>146</v>
+      </c>
+      <c r="I16">
+        <v>18.972000000000001</v>
+      </c>
+      <c r="J16">
+        <v>188.67</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1.1998379629629631E-3</v>
+      </c>
+      <c r="L16">
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <f>MATCH(A17,lapchart!B17:U17,0)</f>
-        <v>14</v>
-      </c>
-      <c r="C17">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A17,finalstanding!B:B,0))</f>
-        <v>10</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>99</v>
+      </c>
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E17" t="s">
+        <v>88</v>
       </c>
       <c r="F17">
-        <f>COUNTIF(pitstop!A:A, A17)</f>
-        <v>2</v>
-      </c>
-      <c r="J17" cm="1">
-        <f t="array" ref="J17">IF(F17&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A17=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>12</v>
-      </c>
-      <c r="K17" cm="1">
-        <f t="array" ref="K17">IF(F17&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J17,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A17=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>29</v>
-      </c>
-      <c r="L17" cm="1">
-        <f t="array" ref="L17">IF(F17&lt;3,IF(F17=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K17),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A17=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v>26</v>
+        <v>54</v>
+      </c>
+      <c r="G17" s="1">
+        <v>6.6348171296296291E-2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>146</v>
+      </c>
+      <c r="I17">
+        <v>12.015000000000001</v>
+      </c>
+      <c r="J17">
+        <v>188.27500000000001</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1.1950925925925926E-3</v>
+      </c>
+      <c r="L17">
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
         <v>63</v>
       </c>
-      <c r="B18">
-        <f>MATCH(A18,lapchart!B18:U18,0)</f>
-        <v>17</v>
-      </c>
-      <c r="C18">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A18,finalstanding!B:B,0))</f>
-        <v>17</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" t="s">
+        <v>139</v>
+      </c>
+      <c r="E18" t="s">
+        <v>86</v>
       </c>
       <c r="F18">
-        <f>COUNTIF(pitstop!A:A, A18)</f>
-        <v>1</v>
-      </c>
-      <c r="J18" cm="1">
-        <f t="array" ref="J18">IF(F18&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A18=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>32</v>
-      </c>
-      <c r="K18" cm="1">
-        <f t="array" ref="K18">IF(F18&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J18,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A18=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>23</v>
-      </c>
-      <c r="L18" t="str" cm="1">
-        <f t="array" ref="L18">IF(F18&lt;3,IF(F18=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K18),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A18=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v/>
+        <v>54</v>
+      </c>
+      <c r="G18" s="1">
+        <v>6.6475682870370367E-2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>146</v>
+      </c>
+      <c r="I18">
+        <v>11.016999999999999</v>
+      </c>
+      <c r="J18">
+        <v>187.91300000000001</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1.192986111111111E-3</v>
+      </c>
+      <c r="L18">
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <f>MATCH(A19,lapchart!B19:U19,0)</f>
-        <v>5</v>
-      </c>
-      <c r="C19">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A19,finalstanding!B:B,0))</f>
-        <v>4</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E19" t="s">
+        <v>80</v>
       </c>
       <c r="F19">
-        <f>COUNTIF(pitstop!A:A, A19)</f>
-        <v>1</v>
-      </c>
-      <c r="J19" cm="1">
-        <f t="array" ref="J19">IF(F19&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A19=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>29</v>
-      </c>
-      <c r="K19" cm="1">
-        <f t="array" ref="K19">IF(F19&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J19,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A19=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>26</v>
-      </c>
-      <c r="L19" t="str" cm="1">
-        <f t="array" ref="L19">IF(F19&lt;3,IF(F19=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K19),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A19=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v/>
+        <v>53</v>
+      </c>
+      <c r="G19" s="1">
+        <v>6.5474548611111114E-2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>153</v>
+      </c>
+      <c r="I19" t="s">
+        <v>146</v>
+      </c>
+      <c r="J19">
+        <v>187.25200000000001</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1.1853472222222224E-3</v>
+      </c>
+      <c r="L19">
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
         <v>88</v>
       </c>
-      <c r="B20">
-        <f>MATCH(A20,lapchart!B20:U20,0)</f>
-        <v>16</v>
-      </c>
-      <c r="C20">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A20,finalstanding!B:B,0))</f>
-        <v>19</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="C20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" t="s">
+        <v>154</v>
+      </c>
+      <c r="E20" t="s">
+        <v>86</v>
       </c>
       <c r="F20">
-        <f>COUNTIF(pitstop!A:A, A20)</f>
-        <v>1</v>
-      </c>
-      <c r="J20" cm="1">
-        <f t="array" ref="J20">IF(F20&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A20=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>24</v>
-      </c>
-      <c r="K20" cm="1">
-        <f t="array" ref="K20">IF(F20&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J20,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A20=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>31</v>
-      </c>
-      <c r="L20" t="str" cm="1">
-        <f t="array" ref="L20">IF(F20&lt;3,IF(F20=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K20),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A20=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v/>
+        <v>53</v>
+      </c>
+      <c r="G20" s="1">
+        <v>6.5618900462962967E-2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>153</v>
+      </c>
+      <c r="I20">
+        <v>12.472</v>
+      </c>
+      <c r="J20">
+        <v>186.84</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1.2094907407407408E-3</v>
+      </c>
+      <c r="L20">
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>99</v>
+      <c r="A21" t="s">
+        <v>110</v>
       </c>
       <c r="B21">
-        <f>MATCH(A21,lapchart!B21:U21,0)</f>
-        <v>16</v>
-      </c>
-      <c r="C21">
-        <f>INDEX(finalstanding!A:A,MATCH(integrated!A21,finalstanding!B:B,0))</f>
-        <v>16</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" t="s">
+        <v>155</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
       </c>
       <c r="F21">
-        <f>COUNTIF(pitstop!A:A, A21)</f>
-        <v>2</v>
-      </c>
-      <c r="J21" cm="1">
-        <f t="array" ref="J21">IF(F21&lt;1,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A21=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+1),1)))</f>
-        <v>8</v>
-      </c>
-      <c r="K21" cm="1">
-        <f t="array" ref="K21">IF(F21&lt;2,LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-J21,INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A21=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+2),1)))</f>
-        <v>18</v>
-      </c>
-      <c r="L21" cm="1">
-        <f t="array" ref="L21">IF(F21&lt;3,IF(F21=1,"",LOOKUP(2,1/(laptimes!A:A&lt;&gt;""),laptimes!A:A)-K21),INDEX(pitstop!$J$2:$J$100,SMALL(IF(integrated!$A21=pitstop!$A$2:$A$100,ROW(pitstop!$A$2:$A$100)-ROW(pitstop!$A$2)+3),1)))</f>
-        <v>37</v>
+        <v>45</v>
+      </c>
+      <c r="G21" s="1">
+        <v>5.5705196759259258E-2</v>
+      </c>
+      <c r="J21">
+        <v>186.857</v>
+      </c>
+      <c r="K21" s="1">
+        <v>1.1959027777777777E-3</v>
+      </c>
+      <c r="L21">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2386,8 +3753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F0C22B-C035-46D0-BF18-D4B9460A3AFE}">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10056,7 +11423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A798E155-A830-4855-9A5E-DE730D057525}">
   <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
@@ -14880,10 +16247,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18896F0-13FF-4F21-9D1E-CDC6EE342C8B}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14900,7 +16267,7 @@
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -14928,11 +16295,8 @@
       <c r="I1" t="s">
         <v>106</v>
       </c>
-      <c r="J1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -14960,12 +16324,8 @@
       <c r="I2">
         <v>3</v>
       </c>
-      <c r="J2">
-        <f>IF(E2&gt;1,D2-D1,D2)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -14993,12 +16353,8 @@
       <c r="I3">
         <v>4</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J27" si="0">IF(E3&gt;1,D3-D2,D3)</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -15026,12 +16382,8 @@
       <c r="I4">
         <v>3</v>
       </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -15059,12 +16411,8 @@
       <c r="I5">
         <v>3</v>
       </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -15092,12 +16440,8 @@
       <c r="I6">
         <v>4</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -15125,12 +16469,8 @@
       <c r="I7">
         <v>3</v>
       </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -15158,12 +16498,8 @@
       <c r="I8">
         <v>3</v>
       </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10</v>
       </c>
@@ -15191,12 +16527,8 @@
       <c r="I9">
         <v>3</v>
       </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11</v>
       </c>
@@ -15224,12 +16556,8 @@
       <c r="I10">
         <v>3</v>
       </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>16</v>
       </c>
@@ -15257,12 +16585,8 @@
       <c r="I11">
         <v>3</v>
       </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>16</v>
       </c>
@@ -15290,12 +16614,8 @@
       <c r="I12">
         <v>5</v>
       </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>18</v>
       </c>
@@ -15323,12 +16643,8 @@
       <c r="I13">
         <v>3</v>
       </c>
-      <c r="J13">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>18</v>
       </c>
@@ -15356,12 +16672,8 @@
       <c r="I14">
         <v>5</v>
       </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20</v>
       </c>
@@ -15389,12 +16701,8 @@
       <c r="I15">
         <v>3</v>
       </c>
-      <c r="J15">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>23</v>
       </c>
@@ -15422,12 +16730,8 @@
       <c r="I16">
         <v>3</v>
       </c>
-      <c r="J16">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>26</v>
       </c>
@@ -15455,12 +16759,8 @@
       <c r="I17">
         <v>4</v>
       </c>
-      <c r="J17">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>27</v>
       </c>
@@ -15488,12 +16788,8 @@
       <c r="I18">
         <v>4</v>
       </c>
-      <c r="J18">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>33</v>
       </c>
@@ -15521,12 +16817,8 @@
       <c r="I19">
         <v>3</v>
       </c>
-      <c r="J19">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>44</v>
       </c>
@@ -15554,12 +16846,8 @@
       <c r="I20">
         <v>3</v>
       </c>
-      <c r="J20">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>55</v>
       </c>
@@ -15587,12 +16875,8 @@
       <c r="I21">
         <v>3</v>
       </c>
-      <c r="J21">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>55</v>
       </c>
@@ -15620,12 +16904,8 @@
       <c r="I22">
         <v>4</v>
       </c>
-      <c r="J22">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>63</v>
       </c>
@@ -15653,12 +16933,8 @@
       <c r="I23">
         <v>4</v>
       </c>
-      <c r="J23">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>77</v>
       </c>
@@ -15686,12 +16962,8 @@
       <c r="I24">
         <v>3</v>
       </c>
-      <c r="J24">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>88</v>
       </c>
@@ -15719,12 +16991,8 @@
       <c r="I25">
         <v>4</v>
       </c>
-      <c r="J25">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>99</v>
       </c>
@@ -15752,12 +17020,8 @@
       <c r="I26">
         <v>3</v>
       </c>
-      <c r="J26">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>99</v>
       </c>
@@ -15784,10 +17048,6 @@
       </c>
       <c r="I27">
         <v>4</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="0"/>
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -15801,13 +17061,15 @@
   <dimension ref="A1:U60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" customWidth="1"/>
     <col min="13" max="21" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -20781,24 +22043,24 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A8BBA3-10D4-484D-8976-742AE906AB2F}">
-  <dimension ref="A1:H21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69FBA700-90F3-4C47-B520-C32B47F15DD0}">
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -20812,19 +22074,22 @@
         <v>100</v>
       </c>
       <c r="E1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" t="s">
         <v>101</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>102</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -20840,24 +22105,28 @@
         <f ca="1">IFERROR(MATCH(A2,INDIRECT("lapchart!"&amp;B2+1&amp;":"&amp;B2+1),0)-1,"")</f>
         <v>11</v>
       </c>
-      <c r="E2" cm="1">
-        <f t="array" aca="1" ref="E2" ca="1">IFERROR(IF(D2=1,"",INDEX(lapchart!$B:$U,B2+1,D2-1)),"")</f>
+      <c r="E2">
+        <f ca="1">IFERROR(MATCH(A2,INDIRECT("lapchart!"&amp;B2+2&amp;":"&amp;B2+2),0)-1,"")</f>
+        <v>11</v>
+      </c>
+      <c r="F2" cm="1">
+        <f t="array" aca="1" ref="F2" ca="1">IFERROR(IF(D2=1,"",INDEX(lapchart!$B:$U,B2+1,D2-1)),"")</f>
         <v>55</v>
       </c>
-      <c r="F2" t="str">
-        <f ca="1">IFERROR(IF(B2&lt;VLOOKUP(E2,A:B,2),MATCH(E2,INDIRECT("lapchart!"&amp;VLOOKUP(E2,A:B,2)+2&amp;":"&amp;VLOOKUP(E2,A:B,2)+2),0)-1,""),"")</f>
-        <v/>
-      </c>
-      <c r="G2" t="str">
-        <f ca="1">IFERROR(IF(F2&lt;&gt;"",ABS(B2-VLOOKUP(E2,A:B,2)),""),"")</f>
-        <v/>
-      </c>
-      <c r="H2" t="str">
-        <f ca="1">IFERROR(F2-D2,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <f t="shared" ref="G2:G21" ca="1" si="0">IFERROR(VLOOKUP(F2,A:E,5),"")</f>
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <f ca="1">IFERROR(IF(G2&lt;&gt;"",B2-VLOOKUP(F2,A:B,2),""),"")</f>
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I21" ca="1" si="1">IFERROR(G2-D2,"")</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -20870,27 +22139,31 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D21" ca="1" si="0">IFERROR(MATCH(A3,INDIRECT("lapchart!"&amp;B3+1&amp;":"&amp;B3+1),0)-1,"")</f>
+        <f t="shared" ref="D3:D21" ca="1" si="2">IFERROR(MATCH(A3,INDIRECT("lapchart!"&amp;B3+1&amp;":"&amp;B3+1),0)-1,"")</f>
         <v>6</v>
       </c>
-      <c r="E3" cm="1">
-        <f t="array" aca="1" ref="E3" ca="1">IFERROR(IF(D3=1,"",INDEX(lapchart!$B:$U,B3+1,D3-1)),"")</f>
+      <c r="E3">
+        <f t="shared" ref="E3:E21" ca="1" si="3">IFERROR(MATCH(A3,INDIRECT("lapchart!"&amp;B3+2&amp;":"&amp;B3+2),0)-1,"")</f>
+        <v>7</v>
+      </c>
+      <c r="F3" cm="1">
+        <f t="array" aca="1" ref="F3" ca="1">IFERROR(IF(D3=1,"",INDEX(lapchart!$B:$U,B3+1,D3-1)),"")</f>
         <v>23</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F21" ca="1" si="1">IFERROR(IF(B3&lt;VLOOKUP(E3,A:B,2),MATCH(E3,INDIRECT("lapchart!"&amp;VLOOKUP(E3,A:B,2)+2&amp;":"&amp;VLOOKUP(E3,A:B,2)+2),0)-1,""),"")</f>
+      <c r="G3">
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G21" ca="1" si="2">IFERROR(IF(F3&lt;&gt;"",ABS(B3-VLOOKUP(E3,A:B,2)),""),"")</f>
-        <v>5</v>
-      </c>
       <c r="H3">
-        <f t="shared" ref="H3:H21" ca="1" si="3">IFERROR(F3-D3,"")</f>
+        <f t="shared" ref="H3:H21" ca="1" si="4">IFERROR(IF(G3&lt;&gt;"",B3-VLOOKUP(F3,A:B,2),""),"")</f>
+        <v>-5</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ca="1" si="1"/>
         <v>-3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -20903,27 +22176,31 @@
         <v>2</v>
       </c>
       <c r="D4">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="F4" cm="1">
+        <f t="array" aca="1" ref="F4" ca="1">IFERROR(IF(D4=1,"",INDEX(lapchart!$B:$U,B4+1,D4-1)),"")</f>
+        <v>16</v>
+      </c>
+      <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E4" cm="1">
-        <f t="array" aca="1" ref="E4" ca="1">IFERROR(IF(D4=1,"",INDEX(lapchart!$B:$U,B4+1,D4-1)),"")</f>
-        <v>16</v>
-      </c>
-      <c r="F4" t="str">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I4">
         <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="G4" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="H4" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
@@ -20936,27 +22213,31 @@
         <v>1</v>
       </c>
       <c r="D5">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="F5" cm="1">
+        <f t="array" aca="1" ref="F5" ca="1">IFERROR(IF(D5=1,"",INDEX(lapchart!$B:$U,B5+1,D5-1)),"")</f>
+        <v>26</v>
+      </c>
+      <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="E5" cm="1">
-        <f t="array" aca="1" ref="E5" ca="1">IFERROR(IF(D5=1,"",INDEX(lapchart!$B:$U,B5+1,D5-1)),"")</f>
-        <v>26</v>
-      </c>
-      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ca="1" si="4"/>
+        <v>-18</v>
+      </c>
+      <c r="I5">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="G5">
-        <f t="shared" ca="1" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="H5">
-        <f t="shared" ca="1" si="3"/>
         <v>-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
@@ -20969,27 +22250,31 @@
         <v>1</v>
       </c>
       <c r="D6">
+        <f t="shared" ca="1" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="F6" cm="1">
+        <f t="array" aca="1" ref="F6" ca="1">IFERROR(IF(D6=1,"",INDEX(lapchart!$B:$U,B6+1,D6-1)),"")</f>
+        <v>26</v>
+      </c>
+      <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="E6" cm="1">
-        <f t="array" aca="1" ref="E6" ca="1">IFERROR(IF(D6=1,"",INDEX(lapchart!$B:$U,B6+1,D6-1)),"")</f>
-        <v>26</v>
-      </c>
-      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="4"/>
+        <v>-22</v>
+      </c>
+      <c r="I6">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="G6">
-        <f t="shared" ca="1" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="H6">
-        <f t="shared" ca="1" si="3"/>
         <v>-5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
@@ -21002,27 +22287,31 @@
         <v>1</v>
       </c>
       <c r="D7">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="F7" cm="1">
+        <f t="array" aca="1" ref="F7" ca="1">IFERROR(IF(D7=1,"",INDEX(lapchart!$B:$U,B7+1,D7-1)),"")</f>
+        <v>11</v>
+      </c>
+      <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E7" cm="1">
-        <f t="array" aca="1" ref="E7" ca="1">IFERROR(IF(D7=1,"",INDEX(lapchart!$B:$U,B7+1,D7-1)),"")</f>
-        <v>11</v>
-      </c>
-      <c r="F7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ca="1" si="4"/>
+        <v>-36</v>
+      </c>
+      <c r="I7">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="G7">
-        <f t="shared" ca="1" si="2"/>
-        <v>36</v>
-      </c>
-      <c r="H7">
-        <f t="shared" ca="1" si="3"/>
         <v>-4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11</v>
       </c>
@@ -21035,27 +22324,31 @@
         <v>1</v>
       </c>
       <c r="D8">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="F8" cm="1">
+        <f t="array" aca="1" ref="F8" ca="1">IFERROR(IF(D8=1,"",INDEX(lapchart!$B:$U,B8+1,D8-1)),"")</f>
+        <v>77</v>
+      </c>
+      <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="E8" cm="1">
-        <f t="array" aca="1" ref="E8" ca="1">IFERROR(IF(D8=1,"",INDEX(lapchart!$B:$U,B8+1,D8-1)),"")</f>
-        <v>77</v>
-      </c>
-      <c r="F8" t="str">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="I8">
         <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="G8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="H8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>16</v>
       </c>
@@ -21068,27 +22361,31 @@
         <v>2</v>
       </c>
       <c r="D9">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="F9" cm="1">
+        <f t="array" aca="1" ref="F9" ca="1">IFERROR(IF(D9=1,"",INDEX(lapchart!$B:$U,B9+1,D9-1)),"")</f>
+        <v>33</v>
+      </c>
+      <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E9" cm="1">
-        <f t="array" aca="1" ref="E9" ca="1">IFERROR(IF(D9=1,"",INDEX(lapchart!$B:$U,B9+1,D9-1)),"")</f>
-        <v>33</v>
-      </c>
-      <c r="F9" t="str">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ca="1" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="I9">
         <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="G9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="H9" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>18</v>
       </c>
@@ -21101,27 +22398,31 @@
         <v>2</v>
       </c>
       <c r="D10">
+        <f t="shared" ca="1" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="F10" cm="1">
+        <f t="array" aca="1" ref="F10" ca="1">IFERROR(IF(D10=1,"",INDEX(lapchart!$B:$U,B10+1,D10-1)),"")</f>
+        <v>63</v>
+      </c>
+      <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="E10" cm="1">
-        <f t="array" aca="1" ref="E10" ca="1">IFERROR(IF(D10=1,"",INDEX(lapchart!$B:$U,B10+1,D10-1)),"")</f>
-        <v>63</v>
-      </c>
-      <c r="F10">
+        <v>16</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ca="1" si="4"/>
+        <v>-9</v>
+      </c>
+      <c r="I10">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="G10">
-        <f t="shared" ca="1" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="H10">
-        <f t="shared" ca="1" si="3"/>
         <v>-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20</v>
       </c>
@@ -21134,27 +22435,31 @@
         <v>1</v>
       </c>
       <c r="D11">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="F11" cm="1">
+        <f t="array" aca="1" ref="F11" ca="1">IFERROR(IF(D11=1,"",INDEX(lapchart!$B:$U,B11+1,D11-1)),"")</f>
+        <v>11</v>
+      </c>
+      <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E11" cm="1">
-        <f t="array" aca="1" ref="E11" ca="1">IFERROR(IF(D11=1,"",INDEX(lapchart!$B:$U,B11+1,D11-1)),"")</f>
-        <v>11</v>
-      </c>
-      <c r="F11">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ca="1" si="4"/>
+        <v>-17</v>
+      </c>
+      <c r="I11">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="G11">
-        <f t="shared" ca="1" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="H11">
-        <f t="shared" ca="1" si="3"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>23</v>
       </c>
@@ -21167,27 +22472,31 @@
         <v>1</v>
       </c>
       <c r="D12">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="F12" cm="1">
+        <f t="array" aca="1" ref="F12" ca="1">IFERROR(IF(D12=1,"",INDEX(lapchart!$B:$U,B12+1,D12-1)),"")</f>
+        <v>5</v>
+      </c>
+      <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E12" cm="1">
-        <f t="array" aca="1" ref="E12" ca="1">IFERROR(IF(D12=1,"",INDEX(lapchart!$B:$U,B12+1,D12-1)),"")</f>
-        <v>5</v>
-      </c>
-      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ca="1" si="4"/>
+        <v>-25</v>
+      </c>
+      <c r="I12">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="G12">
-        <f t="shared" ca="1" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="H12">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>26</v>
       </c>
@@ -21200,27 +22509,31 @@
         <v>1</v>
       </c>
       <c r="D13">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="F13" cm="1">
+        <f t="array" aca="1" ref="F13" ca="1">IFERROR(IF(D13=1,"",INDEX(lapchart!$B:$U,B13+1,D13-1)),"")</f>
+        <v>5</v>
+      </c>
+      <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="E13" cm="1">
-        <f t="array" aca="1" ref="E13" ca="1">IFERROR(IF(D13=1,"",INDEX(lapchart!$B:$U,B13+1,D13-1)),"")</f>
-        <v>5</v>
-      </c>
-      <c r="F13" t="str">
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="I13">
         <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="H13" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>27</v>
       </c>
@@ -21233,27 +22546,31 @@
         <v>1</v>
       </c>
       <c r="D14">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="F14" cm="1">
+        <f t="array" aca="1" ref="F14" ca="1">IFERROR(IF(D14=1,"",INDEX(lapchart!$B:$U,B14+1,D14-1)),"")</f>
+        <v>16</v>
+      </c>
+      <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E14" cm="1">
-        <f t="array" aca="1" ref="E14" ca="1">IFERROR(IF(D14=1,"",INDEX(lapchart!$B:$U,B14+1,D14-1)),"")</f>
-        <v>16</v>
-      </c>
-      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ca="1" si="4"/>
+        <v>-20</v>
+      </c>
+      <c r="I14">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G14">
-        <f t="shared" ca="1" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="H14">
-        <f t="shared" ca="1" si="3"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>33</v>
       </c>
@@ -21266,27 +22583,31 @@
         <v>1</v>
       </c>
       <c r="D15">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F15" cm="1">
+        <f t="array" aca="1" ref="F15" ca="1">IFERROR(IF(D15=1,"",INDEX(lapchart!$B:$U,B15+1,D15-1)),"")</f>
+        <v>44</v>
+      </c>
+      <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E15" cm="1">
-        <f t="array" aca="1" ref="E15" ca="1">IFERROR(IF(D15=1,"",INDEX(lapchart!$B:$U,B15+1,D15-1)),"")</f>
-        <v>44</v>
-      </c>
-      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ca="1" si="4"/>
+        <v>-1</v>
+      </c>
+      <c r="I15">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <f t="shared" ca="1" si="3"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>44</v>
       </c>
@@ -21299,27 +22620,31 @@
         <v>1</v>
       </c>
       <c r="D16">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F16" t="str" cm="1">
+        <f t="array" aca="1" ref="F16" ca="1">IFERROR(IF(D16=1,"",INDEX(lapchart!$B:$U,B16+1,D16-1)),"")</f>
+        <v/>
+      </c>
+      <c r="G16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E16" t="str" cm="1">
-        <f t="array" aca="1" ref="E16" ca="1">IFERROR(IF(D16=1,"",INDEX(lapchart!$B:$U,B16+1,D16-1)),"")</f>
         <v/>
       </c>
-      <c r="F16" t="str">
+      <c r="H16" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="I16" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="G16" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="H16" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>55</v>
       </c>
@@ -21332,27 +22657,31 @@
         <v>2</v>
       </c>
       <c r="D17">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="F17" cm="1">
+        <f t="array" aca="1" ref="F17" ca="1">IFERROR(IF(D17=1,"",INDEX(lapchart!$B:$U,B17+1,D17-1)),"")</f>
+        <v>27</v>
+      </c>
+      <c r="G17">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="E17" cm="1">
-        <f t="array" aca="1" ref="E17" ca="1">IFERROR(IF(D17=1,"",INDEX(lapchart!$B:$U,B17+1,D17-1)),"")</f>
-        <v>27</v>
-      </c>
-      <c r="F17" t="str">
+        <v>7</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ca="1" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="G17" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="H17" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>63</v>
       </c>
@@ -21365,27 +22694,31 @@
         <v>1</v>
       </c>
       <c r="D18">
+        <f t="shared" ca="1" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ca="1" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="F18" cm="1">
+        <f t="array" aca="1" ref="F18" ca="1">IFERROR(IF(D18=1,"",INDEX(lapchart!$B:$U,B18+1,D18-1)),"")</f>
+        <v>8</v>
+      </c>
+      <c r="G18">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="E18" cm="1">
-        <f t="array" aca="1" ref="E18" ca="1">IFERROR(IF(D18=1,"",INDEX(lapchart!$B:$U,B18+1,D18-1)),"")</f>
-        <v>8</v>
-      </c>
-      <c r="F18" t="str">
+        <v>15</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ca="1" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="G18" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="H18" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>77</v>
       </c>
@@ -21398,27 +22731,31 @@
         <v>1</v>
       </c>
       <c r="D19">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F19" cm="1">
+        <f t="array" aca="1" ref="F19" ca="1">IFERROR(IF(D19=1,"",INDEX(lapchart!$B:$U,B19+1,D19-1)),"")</f>
+        <v>33</v>
+      </c>
+      <c r="G19">
         <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ca="1" si="4"/>
         <v>4</v>
       </c>
-      <c r="E19" cm="1">
-        <f t="array" aca="1" ref="E19" ca="1">IFERROR(IF(D19=1,"",INDEX(lapchart!$B:$U,B19+1,D19-1)),"")</f>
-        <v>33</v>
-      </c>
-      <c r="F19" t="str">
+      <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="G19" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="H19" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>88</v>
       </c>
@@ -21431,27 +22768,31 @@
         <v>1</v>
       </c>
       <c r="D20">
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="F20" cm="1">
+        <f t="array" aca="1" ref="F20" ca="1">IFERROR(IF(D20=1,"",INDEX(lapchart!$B:$U,B20+1,D20-1)),"")</f>
+        <v>7</v>
+      </c>
+      <c r="G20">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="E20" cm="1">
-        <f t="array" aca="1" ref="E20" ca="1">IFERROR(IF(D20=1,"",INDEX(lapchart!$B:$U,B20+1,D20-1)),"")</f>
-        <v>7</v>
-      </c>
-      <c r="F20" t="str">
+        <v>9</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="I20">
         <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="G20" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="H20" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>99</v>
       </c>
@@ -21464,24 +22805,28 @@
         <v>2</v>
       </c>
       <c r="D21">
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ca="1" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="F21" cm="1">
+        <f t="array" aca="1" ref="F21" ca="1">IFERROR(IF(D21=1,"",INDEX(lapchart!$B:$U,B21+1,D21-1)),"")</f>
+        <v>7</v>
+      </c>
+      <c r="G21">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="E21" cm="1">
-        <f t="array" aca="1" ref="E21" ca="1">IFERROR(IF(D21=1,"",INDEX(lapchart!$B:$U,B21+1,D21-1)),"")</f>
-        <v>7</v>
-      </c>
-      <c r="F21" t="str">
+        <v>9</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="I21">
         <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="G21" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="H21" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>-6</v>
       </c>
     </row>
   </sheetData>
@@ -21505,23 +22850,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
         <v>122</v>
-      </c>
-      <c r="B1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
         <v>124</v>
-      </c>
-      <c r="B2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" s="8">
         <v>0.55000000000000004</v>
@@ -21529,18 +22874,18 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" t="s">
         <v>127</v>
-      </c>
-      <c r="B4" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" t="s">
         <v>129</v>
-      </c>
-      <c r="B5" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -21553,15 +22898,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462B709E-4F89-4A2D-8419-CE543F9C2CEC}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1">
         <v>10.7</v>

</xml_diff>